<commit_message>
Updated Sprint 2 Backlog Burndown Chart
Updated Sprint 2 Backlog Burndown Chart to reflect all progress made during the sprint
</commit_message>
<xml_diff>
--- a/sprints/sprint2/Sprint 2 Backlog Burndown.xlsx
+++ b/sprints/sprint2/Sprint 2 Backlog Burndown.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="44">
   <si>
     <t>Related User Story</t>
   </si>
@@ -43,46 +43,49 @@
     <t>Data Storage</t>
   </si>
   <si>
-    <t>Create Server</t>
+    <t>Develop server</t>
   </si>
   <si>
     <t>Team</t>
   </si>
   <si>
-    <t>Develop server data storage functionality</t>
+    <t>Develop client</t>
+  </si>
+  <si>
+    <t>Develop functionality to store employee credentials on server</t>
+  </si>
+  <si>
+    <t>Brianna</t>
   </si>
   <si>
     <t>Manage Employee Requests</t>
   </si>
   <si>
-    <t>Create employee requests UI</t>
+    <t>Create UI for viewing current requests for employee</t>
   </si>
   <si>
     <t>Destiny</t>
   </si>
   <si>
-    <t>Develop employee requests functionality</t>
+    <t>Create UI for adding a new work request</t>
+  </si>
+  <si>
+    <t>Develop functionality for adding a new work request</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Destiny </t>
   </si>
   <si>
     <t>Create Employee requests feature wireframe and documentation</t>
   </si>
   <si>
-    <t>Edit Employee Profile</t>
+    <t>Employee Clockin</t>
   </si>
   <si>
-    <t>Develop Editing functionality for employee profile</t>
+    <t>Create UI for viewing multiple clockins a day</t>
   </si>
   <si>
-    <t>Brianna</t>
-  </si>
-  <si>
-    <t>See Employee Work Schedule</t>
-  </si>
-  <si>
-    <t>Create work schedule UI</t>
-  </si>
-  <si>
-    <t>Develop Editing functionality for employee hours</t>
+    <t>Refactor Clockin feature to support muliple clockins</t>
   </si>
   <si>
     <t>View Hours</t>
@@ -91,19 +94,19 @@
     <t>Add hours worked to landing page UI</t>
   </si>
   <si>
-    <t xml:space="preserve"> Hr wants to see employees schedule and hrs worked</t>
+    <t>Hr landing page refactoring</t>
   </si>
   <si>
-    <t>Display the schedule and hrs worked of the selected employee</t>
+    <t>Refactor the distribution of the button in the page, textfields, etc</t>
   </si>
   <si>
     <t>Miguel</t>
   </si>
   <si>
-    <t>Hr wants to edit employees schedule and payment</t>
+    <t>Create a UI for the add employee page functionality</t>
   </si>
   <si>
-    <t>Develop editing functionality for the schedule and payment of the selected employee</t>
+    <t>Develop functionality for adding a new employee profile</t>
   </si>
   <si>
     <t>Hr wants to interact with the employees requests</t>
@@ -115,22 +118,28 @@
     <t>Develop editing/respond functionality</t>
   </si>
   <si>
-    <t>Schedule meetings with HR</t>
+    <t>Log Out</t>
   </si>
   <si>
-    <t>Develop UI for employee meeting schedule</t>
+    <t>Add Log Out Functionality</t>
   </si>
   <si>
     <t>Fernando</t>
   </si>
   <si>
-    <t>Calculate Weekly Pay</t>
+    <t>Documentation</t>
   </si>
   <si>
-    <t>Develop functionality to calculate pay</t>
+    <t>Update Class Diagram to include new functionality</t>
   </si>
   <si>
-    <t>Develop functionality to schedule meeting</t>
+    <t>Update Use Case Diagram to include new functionality</t>
+  </si>
+  <si>
+    <t>Add Use Cases for New Functionality</t>
+  </si>
+  <si>
+    <t>Update system wireframe to include new functionality UI</t>
   </si>
   <si>
     <t>Estimate Totals</t>
@@ -140,11 +149,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b/>
@@ -153,6 +163,11 @@
       <name val="Calibri"/>
     </font>
     <font/>
+    <font>
+      <sz val="11.0"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+    </font>
     <font>
       <sz val="11.0"/>
       <color rgb="FF000000"/>
@@ -166,6 +181,7 @@
     <font>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="7">
@@ -246,7 +262,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -273,31 +289,34 @@
     </xf>
     <xf borderId="7" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="1" fillId="3" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="2" fillId="4" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="2" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="2" fillId="4" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="2" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="2" fillId="5" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="2" fillId="5" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="4" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="2" fillId="5" fontId="0" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="0" fillId="4" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="4" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
-    <xf borderId="2" fillId="4" fontId="0" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="2" fillId="4" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="2" fillId="4" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="2" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
+    <xf borderId="2" fillId="5" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="2" fillId="6" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="right" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="2" fillId="6" fontId="0" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="2" fillId="6" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -358,17 +377,17 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$27:$H$27</c:f>
+              <c:f>Sheet1!$D$29:$H$29</c:f>
               <c:numCache/>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="1858832309"/>
-        <c:axId val="453821888"/>
+        <c:axId val="1041989289"/>
+        <c:axId val="1846411049"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1858832309"/>
+        <c:axId val="1041989289"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -420,10 +439,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="453821888"/>
+        <c:crossAx val="1846411049"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="453821888"/>
+        <c:axId val="1846411049"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -487,7 +506,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1858832309"/>
+        <c:crossAx val="1041989289"/>
       </c:valAx>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
@@ -793,13 +812,23 @@
       <c r="C4" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="12"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
-    </row>
-    <row r="5" ht="21.75" customHeight="1">
+      <c r="D4" s="12">
+        <v>5.0</v>
+      </c>
+      <c r="E4" s="14">
+        <v>2.0</v>
+      </c>
+      <c r="F4" s="14">
+        <v>0.0</v>
+      </c>
+      <c r="G4" s="14">
+        <v>0.0</v>
+      </c>
+      <c r="H4" s="14">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="5">
       <c r="A5" s="12" t="s">
         <v>9</v>
       </c>
@@ -809,3278 +838,3484 @@
       <c r="C5" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="12"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14"/>
-    </row>
-    <row r="6">
+      <c r="D5" s="12">
+        <v>6.0</v>
+      </c>
+      <c r="E5" s="14">
+        <v>0.0</v>
+      </c>
+      <c r="F5" s="14">
+        <v>0.0</v>
+      </c>
+      <c r="G5" s="14">
+        <v>0.0</v>
+      </c>
+      <c r="H5" s="14">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6" ht="30.0" customHeight="1">
       <c r="A6" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="15" t="s">
+      <c r="C6" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="D6" s="12">
+        <v>10.0</v>
+      </c>
+      <c r="E6" s="14">
+        <v>4.0</v>
+      </c>
+      <c r="F6" s="14">
+        <v>2.0</v>
+      </c>
+      <c r="G6" s="14">
+        <v>1.0</v>
+      </c>
+      <c r="H6" s="14">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="12" t="s">
         <v>15</v>
-      </c>
-      <c r="D6" s="12">
-        <v>2.0</v>
-      </c>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
-    </row>
-    <row r="7" ht="30.0" customHeight="1">
-      <c r="A7" s="12" t="s">
-        <v>13</v>
       </c>
       <c r="B7" s="15" t="s">
         <v>16</v>
       </c>
       <c r="C7" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="12">
+        <v>2.0</v>
+      </c>
+      <c r="E7" s="14">
+        <v>0.0</v>
+      </c>
+      <c r="F7" s="14">
+        <v>0.0</v>
+      </c>
+      <c r="G7" s="14">
+        <v>0.0</v>
+      </c>
+      <c r="H7" s="14">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="12">
-        <v>20.0</v>
-      </c>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14"/>
-    </row>
-    <row r="8">
-      <c r="A8" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" s="13" t="s">
+      <c r="B8" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="D8" s="12">
+        <v>2.0</v>
+      </c>
+      <c r="E8" s="14">
+        <v>2.0</v>
+      </c>
+      <c r="F8" s="14">
+        <v>0.0</v>
+      </c>
+      <c r="G8" s="14">
+        <v>0.0</v>
+      </c>
+      <c r="H8" s="14">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="12">
-        <v>5.0</v>
-      </c>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
-      <c r="H8" s="14"/>
-    </row>
-    <row r="9">
-      <c r="A9" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" s="13" t="s">
+      <c r="B9" s="15" t="s">
         <v>19</v>
       </c>
       <c r="C9" s="12" t="s">
         <v>20</v>
       </c>
       <c r="D9" s="12">
-        <v>7.0</v>
-      </c>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="14"/>
+        <v>5.0</v>
+      </c>
+      <c r="E9" s="14">
+        <v>5.0</v>
+      </c>
+      <c r="F9" s="14">
+        <v>2.0</v>
+      </c>
+      <c r="G9" s="14">
+        <v>1.0</v>
+      </c>
+      <c r="H9" s="14">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="13" t="s">
-        <v>22</v>
-      </c>
       <c r="C10" s="12" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D10" s="12">
         <v>3.0</v>
       </c>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="14"/>
+      <c r="E10" s="14">
+        <v>2.0</v>
+      </c>
+      <c r="F10" s="14">
+        <v>1.0</v>
+      </c>
+      <c r="G10" s="14">
+        <v>0.0</v>
+      </c>
+      <c r="H10" s="14">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="12" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B11" s="13" t="s">
         <v>23</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="D11" s="12">
-        <v>7.0</v>
-      </c>
-      <c r="E11" s="16"/>
-      <c r="F11" s="16"/>
-      <c r="G11" s="16"/>
-      <c r="H11" s="16"/>
+        <v>2.0</v>
+      </c>
+      <c r="E11" s="14">
+        <v>2.0</v>
+      </c>
+      <c r="F11" s="14">
+        <v>2.0</v>
+      </c>
+      <c r="G11" s="14">
+        <v>0.0</v>
+      </c>
+      <c r="H11" s="14">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B12" s="13" t="s">
-        <v>25</v>
-      </c>
       <c r="C12" s="12" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="D12" s="12">
-        <v>2.0</v>
-      </c>
-      <c r="E12" s="16"/>
-      <c r="F12" s="16"/>
-      <c r="G12" s="16"/>
-      <c r="H12" s="16"/>
+        <v>5.0</v>
+      </c>
+      <c r="E12" s="14">
+        <v>3.0</v>
+      </c>
+      <c r="F12" s="14">
+        <v>3.0</v>
+      </c>
+      <c r="G12" s="14">
+        <v>0.0</v>
+      </c>
+      <c r="H12" s="14">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="B13" s="13" t="s">
-        <v>27</v>
-      </c>
       <c r="C13" s="12" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="D13" s="12">
-        <v>5.0</v>
-      </c>
-      <c r="E13" s="16"/>
-      <c r="F13" s="16"/>
-      <c r="G13" s="16"/>
-      <c r="H13" s="16"/>
+        <v>1.0</v>
+      </c>
+      <c r="E13" s="14">
+        <v>1.0</v>
+      </c>
+      <c r="F13" s="14">
+        <v>1.0</v>
+      </c>
+      <c r="G13" s="14">
+        <v>0.0</v>
+      </c>
+      <c r="H13" s="14">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="B14" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="C14" s="12" t="s">
-        <v>28</v>
-      </c>
       <c r="D14" s="12">
-        <v>5.0</v>
-      </c>
-      <c r="E14" s="16"/>
-      <c r="F14" s="16"/>
-      <c r="G14" s="16"/>
-      <c r="H14" s="16"/>
+        <v>1.0</v>
+      </c>
+      <c r="E14" s="14">
+        <v>0.0</v>
+      </c>
+      <c r="F14" s="14">
+        <v>0.0</v>
+      </c>
+      <c r="G14" s="14">
+        <v>0.0</v>
+      </c>
+      <c r="H14" s="14">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="12" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D15" s="12">
-        <v>3.0</v>
-      </c>
-      <c r="E15" s="16"/>
-      <c r="F15" s="16"/>
-      <c r="G15" s="16"/>
-      <c r="H15" s="16"/>
+        <v>2.0</v>
+      </c>
+      <c r="E15" s="14">
+        <v>0.0</v>
+      </c>
+      <c r="F15" s="14">
+        <v>0.0</v>
+      </c>
+      <c r="G15" s="14">
+        <v>0.0</v>
+      </c>
+      <c r="H15" s="14">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="B16" s="13" t="s">
-        <v>33</v>
-      </c>
       <c r="C16" s="12" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D16" s="12">
-        <v>8.0</v>
-      </c>
-      <c r="E16" s="16"/>
-      <c r="F16" s="16"/>
-      <c r="G16" s="16"/>
-      <c r="H16" s="16"/>
+        <v>5.0</v>
+      </c>
+      <c r="E16" s="14">
+        <v>4.0</v>
+      </c>
+      <c r="F16" s="14">
+        <v>1.0</v>
+      </c>
+      <c r="G16" s="14">
+        <v>1.0</v>
+      </c>
+      <c r="H16" s="14">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="D17" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="E17" s="14">
+        <v>1.0</v>
+      </c>
+      <c r="F17" s="14">
+        <v>1.0</v>
+      </c>
+      <c r="G17" s="14">
+        <v>0.3</v>
+      </c>
+      <c r="H17" s="14">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="B17" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="C17" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="D17" s="12">
+      <c r="C18" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="D18" s="12">
+        <v>4.0</v>
+      </c>
+      <c r="E18" s="14">
+        <v>4.0</v>
+      </c>
+      <c r="F18" s="14">
+        <v>4.0</v>
+      </c>
+      <c r="G18" s="14">
         <v>2.0</v>
       </c>
-      <c r="E17" s="16"/>
-      <c r="F17" s="16"/>
-      <c r="G17" s="16"/>
-      <c r="H17" s="16"/>
-    </row>
-    <row r="18">
-      <c r="A18" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="B18" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="C18" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="D18" s="12">
-        <v>2.0</v>
-      </c>
-      <c r="E18" s="16"/>
-      <c r="F18" s="16"/>
-      <c r="G18" s="16"/>
-      <c r="H18" s="16"/>
+      <c r="H18" s="14">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="12" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B19" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="D19" s="12">
+        <v>2.0</v>
+      </c>
+      <c r="E19" s="14">
+        <v>0.0</v>
+      </c>
+      <c r="F19" s="14">
+        <v>0.0</v>
+      </c>
+      <c r="G19" s="14">
+        <v>0.0</v>
+      </c>
+      <c r="H19" s="14">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="C19" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="D19" s="12">
-        <v>4.0</v>
-      </c>
-      <c r="E19" s="16"/>
-      <c r="F19" s="16"/>
-      <c r="G19" s="16"/>
-      <c r="H19" s="16"/>
-    </row>
-    <row r="20">
-      <c r="A20" s="18"/>
-      <c r="B20" s="19"/>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="16"/>
-      <c r="F20" s="16"/>
-      <c r="G20" s="16"/>
-      <c r="H20" s="16"/>
-    </row>
-    <row r="21" ht="15.75" customHeight="1">
-      <c r="A21" s="18"/>
-      <c r="B21" s="19"/>
-      <c r="C21" s="18"/>
-      <c r="D21" s="18"/>
-      <c r="E21" s="16"/>
-      <c r="F21" s="16"/>
-      <c r="G21" s="16"/>
-      <c r="H21" s="16"/>
-    </row>
-    <row r="22" ht="15.75" customHeight="1">
-      <c r="A22" s="18"/>
-      <c r="B22" s="19"/>
-      <c r="C22" s="18"/>
-      <c r="D22" s="18"/>
-      <c r="E22" s="16"/>
-      <c r="F22" s="16"/>
-      <c r="G22" s="16"/>
-      <c r="H22" s="16"/>
+      <c r="C20" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="D20" s="12">
+        <v>3.0</v>
+      </c>
+      <c r="E20" s="14">
+        <v>3.0</v>
+      </c>
+      <c r="F20" s="14">
+        <v>1.0</v>
+      </c>
+      <c r="G20" s="14">
+        <v>0.0</v>
+      </c>
+      <c r="H20" s="14">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="B21" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="D21" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="E21" s="14">
+        <v>1.0</v>
+      </c>
+      <c r="F21" s="14">
+        <v>1.0</v>
+      </c>
+      <c r="G21" s="14">
+        <v>1.0</v>
+      </c>
+      <c r="H21" s="14">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="B22" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="D22" s="12">
+        <v>5.0</v>
+      </c>
+      <c r="E22" s="14">
+        <v>5.0</v>
+      </c>
+      <c r="F22" s="14">
+        <v>3.0</v>
+      </c>
+      <c r="G22" s="14">
+        <v>0.0</v>
+      </c>
+      <c r="H22" s="14">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="23" ht="15.75" customHeight="1">
-      <c r="A23" s="18"/>
-      <c r="B23" s="19"/>
-      <c r="C23" s="18"/>
-      <c r="D23" s="18"/>
-      <c r="E23" s="16"/>
-      <c r="F23" s="16"/>
-      <c r="G23" s="16"/>
-      <c r="H23" s="16"/>
+      <c r="A23" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="B23" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="D23" s="12">
+        <v>3.0</v>
+      </c>
+      <c r="E23" s="14">
+        <v>3.0</v>
+      </c>
+      <c r="F23" s="14">
+        <v>0.0</v>
+      </c>
+      <c r="G23" s="14">
+        <v>0.0</v>
+      </c>
+      <c r="H23" s="14">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="24" ht="15.75" customHeight="1">
       <c r="A24" s="18"/>
       <c r="B24" s="19"/>
       <c r="C24" s="18"/>
       <c r="D24" s="18"/>
-      <c r="E24" s="16"/>
-      <c r="F24" s="16"/>
-      <c r="G24" s="16"/>
-      <c r="H24" s="16"/>
+      <c r="E24" s="20"/>
+      <c r="F24" s="20"/>
+      <c r="G24" s="20"/>
+      <c r="H24" s="20"/>
     </row>
     <row r="25" ht="15.75" customHeight="1">
       <c r="A25" s="18"/>
       <c r="B25" s="19"/>
       <c r="C25" s="18"/>
       <c r="D25" s="18"/>
-      <c r="E25" s="16"/>
-      <c r="F25" s="16"/>
-      <c r="G25" s="16"/>
-      <c r="H25" s="16"/>
+      <c r="E25" s="20"/>
+      <c r="F25" s="20"/>
+      <c r="G25" s="20"/>
+      <c r="H25" s="20"/>
     </row>
     <row r="26" ht="15.75" customHeight="1">
       <c r="A26" s="18"/>
       <c r="B26" s="19"/>
       <c r="C26" s="18"/>
       <c r="D26" s="18"/>
-      <c r="E26" s="16"/>
-      <c r="F26" s="16"/>
-      <c r="G26" s="16"/>
-      <c r="H26" s="16"/>
+      <c r="E26" s="20"/>
+      <c r="F26" s="20"/>
+      <c r="G26" s="20"/>
+      <c r="H26" s="20"/>
     </row>
     <row r="27" ht="15.75" customHeight="1">
-      <c r="B27" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="C27" s="21"/>
-      <c r="D27" s="21">
-        <f t="shared" ref="D27:H27" si="1">SUM(D4:D26)</f>
-        <v>75</v>
-      </c>
-      <c r="E27" s="21">
+      <c r="A27" s="18"/>
+      <c r="B27" s="19"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="20"/>
+      <c r="F27" s="20"/>
+      <c r="G27" s="20"/>
+      <c r="H27" s="20"/>
+    </row>
+    <row r="28" ht="15.75" customHeight="1">
+      <c r="A28" s="18"/>
+      <c r="B28" s="19"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="20"/>
+      <c r="F28" s="20"/>
+      <c r="G28" s="20"/>
+      <c r="H28" s="20"/>
+    </row>
+    <row r="29" ht="15.75" customHeight="1">
+      <c r="B29" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="C29" s="22"/>
+      <c r="D29" s="22">
+        <f t="shared" ref="D29:H29" si="1">SUM(D4:D28)</f>
+        <v>68</v>
+      </c>
+      <c r="E29" s="22">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F27" s="21">
+        <v>42</v>
+      </c>
+      <c r="F29" s="22">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G27" s="21">
+        <v>22</v>
+      </c>
+      <c r="G29" s="22">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H27" s="21">
+        <v>6.3</v>
+      </c>
+      <c r="H29" s="22">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" ht="15.75" customHeight="1">
-      <c r="B28" s="22"/>
-    </row>
-    <row r="29" ht="15.75" customHeight="1">
-      <c r="B29" s="22"/>
+        <v>0.3</v>
+      </c>
     </row>
     <row r="30" ht="15.75" customHeight="1">
-      <c r="B30" s="22"/>
+      <c r="B30" s="23"/>
     </row>
     <row r="31" ht="15.75" customHeight="1">
-      <c r="B31" s="22"/>
+      <c r="B31" s="23"/>
     </row>
     <row r="32" ht="15.75" customHeight="1">
-      <c r="B32" s="22"/>
+      <c r="B32" s="23"/>
     </row>
     <row r="33" ht="15.75" customHeight="1">
-      <c r="B33" s="22"/>
+      <c r="B33" s="23"/>
     </row>
     <row r="34" ht="15.75" customHeight="1">
-      <c r="B34" s="22"/>
+      <c r="B34" s="23"/>
     </row>
     <row r="35" ht="15.75" customHeight="1">
-      <c r="B35" s="22"/>
+      <c r="B35" s="23"/>
     </row>
     <row r="36" ht="15.75" customHeight="1">
-      <c r="B36" s="22"/>
+      <c r="B36" s="23"/>
     </row>
     <row r="37" ht="15.75" customHeight="1">
-      <c r="B37" s="22"/>
+      <c r="B37" s="23"/>
     </row>
     <row r="38" ht="15.75" customHeight="1">
-      <c r="B38" s="22"/>
+      <c r="B38" s="23"/>
     </row>
     <row r="39" ht="15.75" customHeight="1">
-      <c r="B39" s="22"/>
+      <c r="B39" s="23"/>
     </row>
     <row r="40" ht="15.75" customHeight="1">
-      <c r="B40" s="22"/>
+      <c r="B40" s="23"/>
     </row>
     <row r="41" ht="15.75" customHeight="1">
-      <c r="B41" s="22"/>
+      <c r="B41" s="23"/>
     </row>
     <row r="42" ht="15.75" customHeight="1">
-      <c r="B42" s="22"/>
+      <c r="B42" s="23"/>
     </row>
     <row r="43" ht="15.75" customHeight="1">
-      <c r="B43" s="22"/>
+      <c r="B43" s="23"/>
     </row>
     <row r="44" ht="15.75" customHeight="1">
-      <c r="B44" s="22"/>
+      <c r="B44" s="23"/>
     </row>
     <row r="45" ht="15.75" customHeight="1">
-      <c r="B45" s="22"/>
+      <c r="B45" s="23"/>
     </row>
     <row r="46" ht="15.75" customHeight="1">
-      <c r="B46" s="22"/>
+      <c r="B46" s="23"/>
     </row>
     <row r="47" ht="15.75" customHeight="1">
-      <c r="B47" s="22"/>
+      <c r="B47" s="23"/>
     </row>
     <row r="48" ht="15.75" customHeight="1">
-      <c r="B48" s="22"/>
+      <c r="B48" s="23"/>
     </row>
     <row r="49" ht="15.75" customHeight="1">
-      <c r="B49" s="22"/>
+      <c r="B49" s="23"/>
     </row>
     <row r="50" ht="15.75" customHeight="1">
-      <c r="B50" s="22"/>
+      <c r="B50" s="23"/>
     </row>
     <row r="51" ht="15.75" customHeight="1">
-      <c r="B51" s="22"/>
+      <c r="B51" s="23"/>
     </row>
     <row r="52" ht="15.75" customHeight="1">
-      <c r="B52" s="22"/>
+      <c r="B52" s="23"/>
     </row>
     <row r="53" ht="15.75" customHeight="1">
-      <c r="B53" s="22"/>
+      <c r="B53" s="23"/>
     </row>
     <row r="54" ht="15.75" customHeight="1">
-      <c r="B54" s="22"/>
+      <c r="B54" s="23"/>
     </row>
     <row r="55" ht="15.75" customHeight="1">
-      <c r="B55" s="22"/>
+      <c r="B55" s="23"/>
     </row>
     <row r="56" ht="15.75" customHeight="1">
-      <c r="B56" s="22"/>
+      <c r="B56" s="23"/>
     </row>
     <row r="57" ht="15.75" customHeight="1">
-      <c r="B57" s="22"/>
+      <c r="B57" s="23"/>
     </row>
     <row r="58" ht="15.75" customHeight="1">
-      <c r="B58" s="22"/>
+      <c r="B58" s="23"/>
     </row>
     <row r="59" ht="15.75" customHeight="1">
-      <c r="B59" s="22"/>
+      <c r="B59" s="23"/>
     </row>
     <row r="60" ht="15.75" customHeight="1">
-      <c r="B60" s="22"/>
+      <c r="B60" s="23"/>
     </row>
     <row r="61" ht="15.75" customHeight="1">
-      <c r="B61" s="22"/>
+      <c r="B61" s="23"/>
     </row>
     <row r="62" ht="15.75" customHeight="1">
-      <c r="B62" s="22"/>
+      <c r="B62" s="23"/>
     </row>
     <row r="63" ht="15.75" customHeight="1">
-      <c r="B63" s="22"/>
+      <c r="B63" s="23"/>
     </row>
     <row r="64" ht="15.75" customHeight="1">
-      <c r="B64" s="22"/>
+      <c r="B64" s="23"/>
     </row>
     <row r="65" ht="15.75" customHeight="1">
-      <c r="B65" s="22"/>
+      <c r="B65" s="23"/>
     </row>
     <row r="66" ht="15.75" customHeight="1">
-      <c r="B66" s="22"/>
+      <c r="B66" s="23"/>
     </row>
     <row r="67" ht="15.75" customHeight="1">
-      <c r="B67" s="22"/>
+      <c r="B67" s="23"/>
     </row>
     <row r="68" ht="15.75" customHeight="1">
-      <c r="B68" s="22"/>
+      <c r="B68" s="23"/>
     </row>
     <row r="69" ht="15.75" customHeight="1">
-      <c r="B69" s="22"/>
+      <c r="B69" s="23"/>
     </row>
     <row r="70" ht="15.75" customHeight="1">
-      <c r="B70" s="22"/>
+      <c r="B70" s="23"/>
     </row>
     <row r="71" ht="15.75" customHeight="1">
-      <c r="B71" s="22"/>
+      <c r="B71" s="23"/>
     </row>
     <row r="72" ht="15.75" customHeight="1">
-      <c r="B72" s="22"/>
+      <c r="B72" s="23"/>
     </row>
     <row r="73" ht="15.75" customHeight="1">
-      <c r="B73" s="22"/>
+      <c r="B73" s="23"/>
     </row>
     <row r="74" ht="15.75" customHeight="1">
-      <c r="B74" s="22"/>
+      <c r="B74" s="23"/>
     </row>
     <row r="75" ht="15.75" customHeight="1">
-      <c r="B75" s="22"/>
+      <c r="B75" s="23"/>
     </row>
     <row r="76" ht="15.75" customHeight="1">
-      <c r="B76" s="22"/>
+      <c r="B76" s="23"/>
     </row>
     <row r="77" ht="15.75" customHeight="1">
-      <c r="B77" s="22"/>
+      <c r="B77" s="23"/>
     </row>
     <row r="78" ht="15.75" customHeight="1">
-      <c r="B78" s="22"/>
+      <c r="B78" s="23"/>
     </row>
     <row r="79" ht="15.75" customHeight="1">
-      <c r="B79" s="22"/>
+      <c r="B79" s="23"/>
     </row>
     <row r="80" ht="15.75" customHeight="1">
-      <c r="B80" s="22"/>
+      <c r="B80" s="23"/>
     </row>
     <row r="81" ht="15.75" customHeight="1">
-      <c r="B81" s="22"/>
+      <c r="B81" s="23"/>
     </row>
     <row r="82" ht="15.75" customHeight="1">
-      <c r="B82" s="22"/>
+      <c r="B82" s="23"/>
     </row>
     <row r="83" ht="15.75" customHeight="1">
-      <c r="B83" s="22"/>
+      <c r="B83" s="23"/>
     </row>
     <row r="84" ht="15.75" customHeight="1">
-      <c r="B84" s="22"/>
+      <c r="B84" s="23"/>
     </row>
     <row r="85" ht="15.75" customHeight="1">
-      <c r="B85" s="22"/>
+      <c r="B85" s="23"/>
     </row>
     <row r="86" ht="15.75" customHeight="1">
-      <c r="B86" s="22"/>
+      <c r="B86" s="23"/>
     </row>
     <row r="87" ht="15.75" customHeight="1">
-      <c r="B87" s="22"/>
+      <c r="B87" s="23"/>
     </row>
     <row r="88" ht="15.75" customHeight="1">
-      <c r="B88" s="22"/>
+      <c r="B88" s="23"/>
     </row>
     <row r="89" ht="15.75" customHeight="1">
-      <c r="B89" s="22"/>
+      <c r="B89" s="23"/>
     </row>
     <row r="90" ht="15.75" customHeight="1">
-      <c r="B90" s="22"/>
+      <c r="B90" s="23"/>
     </row>
     <row r="91" ht="15.75" customHeight="1">
-      <c r="B91" s="22"/>
+      <c r="B91" s="23"/>
     </row>
     <row r="92" ht="15.75" customHeight="1">
-      <c r="B92" s="22"/>
+      <c r="B92" s="23"/>
     </row>
     <row r="93" ht="15.75" customHeight="1">
-      <c r="B93" s="22"/>
+      <c r="B93" s="23"/>
     </row>
     <row r="94" ht="15.75" customHeight="1">
-      <c r="B94" s="22"/>
+      <c r="B94" s="23"/>
     </row>
     <row r="95" ht="15.75" customHeight="1">
-      <c r="B95" s="22"/>
+      <c r="B95" s="23"/>
     </row>
     <row r="96" ht="15.75" customHeight="1">
-      <c r="B96" s="22"/>
+      <c r="B96" s="23"/>
     </row>
     <row r="97" ht="15.75" customHeight="1">
-      <c r="B97" s="22"/>
+      <c r="B97" s="23"/>
     </row>
     <row r="98" ht="15.75" customHeight="1">
-      <c r="B98" s="22"/>
+      <c r="B98" s="23"/>
     </row>
     <row r="99" ht="15.75" customHeight="1">
-      <c r="B99" s="22"/>
+      <c r="B99" s="23"/>
     </row>
     <row r="100" ht="15.75" customHeight="1">
-      <c r="B100" s="22"/>
+      <c r="B100" s="23"/>
     </row>
     <row r="101" ht="15.75" customHeight="1">
-      <c r="B101" s="22"/>
+      <c r="B101" s="23"/>
     </row>
     <row r="102" ht="15.75" customHeight="1">
-      <c r="B102" s="22"/>
+      <c r="B102" s="23"/>
     </row>
     <row r="103" ht="15.75" customHeight="1">
-      <c r="B103" s="22"/>
+      <c r="B103" s="23"/>
     </row>
     <row r="104" ht="15.75" customHeight="1">
-      <c r="B104" s="22"/>
+      <c r="B104" s="23"/>
     </row>
     <row r="105" ht="15.75" customHeight="1">
-      <c r="B105" s="22"/>
+      <c r="B105" s="23"/>
     </row>
     <row r="106" ht="15.75" customHeight="1">
-      <c r="B106" s="22"/>
+      <c r="B106" s="23"/>
     </row>
     <row r="107" ht="15.75" customHeight="1">
-      <c r="B107" s="22"/>
+      <c r="B107" s="23"/>
     </row>
     <row r="108" ht="15.75" customHeight="1">
-      <c r="B108" s="22"/>
+      <c r="B108" s="23"/>
     </row>
     <row r="109" ht="15.75" customHeight="1">
-      <c r="B109" s="22"/>
+      <c r="B109" s="23"/>
     </row>
     <row r="110" ht="15.75" customHeight="1">
-      <c r="B110" s="22"/>
+      <c r="B110" s="23"/>
     </row>
     <row r="111" ht="15.75" customHeight="1">
-      <c r="B111" s="22"/>
+      <c r="B111" s="23"/>
     </row>
     <row r="112" ht="15.75" customHeight="1">
-      <c r="B112" s="22"/>
+      <c r="B112" s="23"/>
     </row>
     <row r="113" ht="15.75" customHeight="1">
-      <c r="B113" s="22"/>
+      <c r="B113" s="23"/>
     </row>
     <row r="114" ht="15.75" customHeight="1">
-      <c r="B114" s="22"/>
+      <c r="B114" s="23"/>
     </row>
     <row r="115" ht="15.75" customHeight="1">
-      <c r="B115" s="22"/>
+      <c r="B115" s="23"/>
     </row>
     <row r="116" ht="15.75" customHeight="1">
-      <c r="B116" s="22"/>
+      <c r="B116" s="23"/>
     </row>
     <row r="117" ht="15.75" customHeight="1">
-      <c r="B117" s="22"/>
+      <c r="B117" s="23"/>
     </row>
     <row r="118" ht="15.75" customHeight="1">
-      <c r="B118" s="22"/>
+      <c r="B118" s="23"/>
     </row>
     <row r="119" ht="15.75" customHeight="1">
-      <c r="B119" s="22"/>
+      <c r="B119" s="23"/>
     </row>
     <row r="120" ht="15.75" customHeight="1">
-      <c r="B120" s="22"/>
+      <c r="B120" s="23"/>
     </row>
     <row r="121" ht="15.75" customHeight="1">
-      <c r="B121" s="22"/>
+      <c r="B121" s="23"/>
     </row>
     <row r="122" ht="15.75" customHeight="1">
-      <c r="B122" s="22"/>
+      <c r="B122" s="23"/>
     </row>
     <row r="123" ht="15.75" customHeight="1">
-      <c r="B123" s="22"/>
+      <c r="B123" s="23"/>
     </row>
     <row r="124" ht="15.75" customHeight="1">
-      <c r="B124" s="22"/>
+      <c r="B124" s="23"/>
     </row>
     <row r="125" ht="15.75" customHeight="1">
-      <c r="B125" s="22"/>
+      <c r="B125" s="23"/>
     </row>
     <row r="126" ht="15.75" customHeight="1">
-      <c r="B126" s="22"/>
+      <c r="B126" s="23"/>
     </row>
     <row r="127" ht="15.75" customHeight="1">
-      <c r="B127" s="22"/>
+      <c r="B127" s="23"/>
     </row>
     <row r="128" ht="15.75" customHeight="1">
-      <c r="B128" s="22"/>
+      <c r="B128" s="23"/>
     </row>
     <row r="129" ht="15.75" customHeight="1">
-      <c r="B129" s="22"/>
+      <c r="B129" s="23"/>
     </row>
     <row r="130" ht="15.75" customHeight="1">
-      <c r="B130" s="22"/>
+      <c r="B130" s="23"/>
     </row>
     <row r="131" ht="15.75" customHeight="1">
-      <c r="B131" s="22"/>
+      <c r="B131" s="23"/>
     </row>
     <row r="132" ht="15.75" customHeight="1">
-      <c r="B132" s="22"/>
+      <c r="B132" s="23"/>
     </row>
     <row r="133" ht="15.75" customHeight="1">
-      <c r="B133" s="22"/>
+      <c r="B133" s="23"/>
     </row>
     <row r="134" ht="15.75" customHeight="1">
-      <c r="B134" s="22"/>
+      <c r="B134" s="23"/>
     </row>
     <row r="135" ht="15.75" customHeight="1">
-      <c r="B135" s="22"/>
+      <c r="B135" s="23"/>
     </row>
     <row r="136" ht="15.75" customHeight="1">
-      <c r="B136" s="22"/>
+      <c r="B136" s="23"/>
     </row>
     <row r="137" ht="15.75" customHeight="1">
-      <c r="B137" s="22"/>
+      <c r="B137" s="23"/>
     </row>
     <row r="138" ht="15.75" customHeight="1">
-      <c r="B138" s="22"/>
+      <c r="B138" s="23"/>
     </row>
     <row r="139" ht="15.75" customHeight="1">
-      <c r="B139" s="22"/>
+      <c r="B139" s="23"/>
     </row>
     <row r="140" ht="15.75" customHeight="1">
-      <c r="B140" s="22"/>
+      <c r="B140" s="23"/>
     </row>
     <row r="141" ht="15.75" customHeight="1">
-      <c r="B141" s="22"/>
+      <c r="B141" s="23"/>
     </row>
     <row r="142" ht="15.75" customHeight="1">
-      <c r="B142" s="22"/>
+      <c r="B142" s="23"/>
     </row>
     <row r="143" ht="15.75" customHeight="1">
-      <c r="B143" s="22"/>
+      <c r="B143" s="23"/>
     </row>
     <row r="144" ht="15.75" customHeight="1">
-      <c r="B144" s="22"/>
+      <c r="B144" s="23"/>
     </row>
     <row r="145" ht="15.75" customHeight="1">
-      <c r="B145" s="22"/>
+      <c r="B145" s="23"/>
     </row>
     <row r="146" ht="15.75" customHeight="1">
-      <c r="B146" s="22"/>
+      <c r="B146" s="23"/>
     </row>
     <row r="147" ht="15.75" customHeight="1">
-      <c r="B147" s="22"/>
+      <c r="B147" s="23"/>
     </row>
     <row r="148" ht="15.75" customHeight="1">
-      <c r="B148" s="22"/>
+      <c r="B148" s="23"/>
     </row>
     <row r="149" ht="15.75" customHeight="1">
-      <c r="B149" s="22"/>
+      <c r="B149" s="23"/>
     </row>
     <row r="150" ht="15.75" customHeight="1">
-      <c r="B150" s="22"/>
+      <c r="B150" s="23"/>
     </row>
     <row r="151" ht="15.75" customHeight="1">
-      <c r="B151" s="22"/>
+      <c r="B151" s="23"/>
     </row>
     <row r="152" ht="15.75" customHeight="1">
-      <c r="B152" s="22"/>
+      <c r="B152" s="23"/>
     </row>
     <row r="153" ht="15.75" customHeight="1">
-      <c r="B153" s="22"/>
+      <c r="B153" s="23"/>
     </row>
     <row r="154" ht="15.75" customHeight="1">
-      <c r="B154" s="22"/>
+      <c r="B154" s="23"/>
     </row>
     <row r="155" ht="15.75" customHeight="1">
-      <c r="B155" s="22"/>
+      <c r="B155" s="23"/>
     </row>
     <row r="156" ht="15.75" customHeight="1">
-      <c r="B156" s="22"/>
+      <c r="B156" s="23"/>
     </row>
     <row r="157" ht="15.75" customHeight="1">
-      <c r="B157" s="22"/>
+      <c r="B157" s="23"/>
     </row>
     <row r="158" ht="15.75" customHeight="1">
-      <c r="B158" s="22"/>
+      <c r="B158" s="23"/>
     </row>
     <row r="159" ht="15.75" customHeight="1">
-      <c r="B159" s="22"/>
+      <c r="B159" s="23"/>
     </row>
     <row r="160" ht="15.75" customHeight="1">
-      <c r="B160" s="22"/>
+      <c r="B160" s="23"/>
     </row>
     <row r="161" ht="15.75" customHeight="1">
-      <c r="B161" s="22"/>
+      <c r="B161" s="23"/>
     </row>
     <row r="162" ht="15.75" customHeight="1">
-      <c r="B162" s="22"/>
+      <c r="B162" s="23"/>
     </row>
     <row r="163" ht="15.75" customHeight="1">
-      <c r="B163" s="22"/>
+      <c r="B163" s="23"/>
     </row>
     <row r="164" ht="15.75" customHeight="1">
-      <c r="B164" s="22"/>
+      <c r="B164" s="23"/>
     </row>
     <row r="165" ht="15.75" customHeight="1">
-      <c r="B165" s="22"/>
+      <c r="B165" s="23"/>
     </row>
     <row r="166" ht="15.75" customHeight="1">
-      <c r="B166" s="22"/>
+      <c r="B166" s="23"/>
     </row>
     <row r="167" ht="15.75" customHeight="1">
-      <c r="B167" s="22"/>
+      <c r="B167" s="23"/>
     </row>
     <row r="168" ht="15.75" customHeight="1">
-      <c r="B168" s="22"/>
+      <c r="B168" s="23"/>
     </row>
     <row r="169" ht="15.75" customHeight="1">
-      <c r="B169" s="22"/>
+      <c r="B169" s="23"/>
     </row>
     <row r="170" ht="15.75" customHeight="1">
-      <c r="B170" s="22"/>
+      <c r="B170" s="23"/>
     </row>
     <row r="171" ht="15.75" customHeight="1">
-      <c r="B171" s="22"/>
+      <c r="B171" s="23"/>
     </row>
     <row r="172" ht="15.75" customHeight="1">
-      <c r="B172" s="22"/>
+      <c r="B172" s="23"/>
     </row>
     <row r="173" ht="15.75" customHeight="1">
-      <c r="B173" s="22"/>
+      <c r="B173" s="23"/>
     </row>
     <row r="174" ht="15.75" customHeight="1">
-      <c r="B174" s="22"/>
+      <c r="B174" s="23"/>
     </row>
     <row r="175" ht="15.75" customHeight="1">
-      <c r="B175" s="22"/>
+      <c r="B175" s="23"/>
     </row>
     <row r="176" ht="15.75" customHeight="1">
-      <c r="B176" s="22"/>
+      <c r="B176" s="23"/>
     </row>
     <row r="177" ht="15.75" customHeight="1">
-      <c r="B177" s="22"/>
+      <c r="B177" s="23"/>
     </row>
     <row r="178" ht="15.75" customHeight="1">
-      <c r="B178" s="22"/>
+      <c r="B178" s="23"/>
     </row>
     <row r="179" ht="15.75" customHeight="1">
-      <c r="B179" s="22"/>
+      <c r="B179" s="23"/>
     </row>
     <row r="180" ht="15.75" customHeight="1">
-      <c r="B180" s="22"/>
+      <c r="B180" s="23"/>
     </row>
     <row r="181" ht="15.75" customHeight="1">
-      <c r="B181" s="22"/>
+      <c r="B181" s="23"/>
     </row>
     <row r="182" ht="15.75" customHeight="1">
-      <c r="B182" s="22"/>
+      <c r="B182" s="23"/>
     </row>
     <row r="183" ht="15.75" customHeight="1">
-      <c r="B183" s="22"/>
+      <c r="B183" s="23"/>
     </row>
     <row r="184" ht="15.75" customHeight="1">
-      <c r="B184" s="22"/>
+      <c r="B184" s="23"/>
     </row>
     <row r="185" ht="15.75" customHeight="1">
-      <c r="B185" s="22"/>
+      <c r="B185" s="23"/>
     </row>
     <row r="186" ht="15.75" customHeight="1">
-      <c r="B186" s="22"/>
+      <c r="B186" s="23"/>
     </row>
     <row r="187" ht="15.75" customHeight="1">
-      <c r="B187" s="22"/>
+      <c r="B187" s="23"/>
     </row>
     <row r="188" ht="15.75" customHeight="1">
-      <c r="B188" s="22"/>
+      <c r="B188" s="23"/>
     </row>
     <row r="189" ht="15.75" customHeight="1">
-      <c r="B189" s="22"/>
+      <c r="B189" s="23"/>
     </row>
     <row r="190" ht="15.75" customHeight="1">
-      <c r="B190" s="22"/>
+      <c r="B190" s="23"/>
     </row>
     <row r="191" ht="15.75" customHeight="1">
-      <c r="B191" s="22"/>
+      <c r="B191" s="23"/>
     </row>
     <row r="192" ht="15.75" customHeight="1">
-      <c r="B192" s="22"/>
+      <c r="B192" s="23"/>
     </row>
     <row r="193" ht="15.75" customHeight="1">
-      <c r="B193" s="22"/>
+      <c r="B193" s="23"/>
     </row>
     <row r="194" ht="15.75" customHeight="1">
-      <c r="B194" s="22"/>
+      <c r="B194" s="23"/>
     </row>
     <row r="195" ht="15.75" customHeight="1">
-      <c r="B195" s="22"/>
+      <c r="B195" s="23"/>
     </row>
     <row r="196" ht="15.75" customHeight="1">
-      <c r="B196" s="22"/>
+      <c r="B196" s="23"/>
     </row>
     <row r="197" ht="15.75" customHeight="1">
-      <c r="B197" s="22"/>
+      <c r="B197" s="23"/>
     </row>
     <row r="198" ht="15.75" customHeight="1">
-      <c r="B198" s="22"/>
+      <c r="B198" s="23"/>
     </row>
     <row r="199" ht="15.75" customHeight="1">
-      <c r="B199" s="22"/>
+      <c r="B199" s="23"/>
     </row>
     <row r="200" ht="15.75" customHeight="1">
-      <c r="B200" s="22"/>
+      <c r="B200" s="23"/>
     </row>
     <row r="201" ht="15.75" customHeight="1">
-      <c r="B201" s="22"/>
+      <c r="B201" s="23"/>
     </row>
     <row r="202" ht="15.75" customHeight="1">
-      <c r="B202" s="22"/>
+      <c r="B202" s="23"/>
     </row>
     <row r="203" ht="15.75" customHeight="1">
-      <c r="B203" s="22"/>
+      <c r="B203" s="23"/>
     </row>
     <row r="204" ht="15.75" customHeight="1">
-      <c r="B204" s="22"/>
+      <c r="B204" s="23"/>
     </row>
     <row r="205" ht="15.75" customHeight="1">
-      <c r="B205" s="22"/>
+      <c r="B205" s="23"/>
     </row>
     <row r="206" ht="15.75" customHeight="1">
-      <c r="B206" s="22"/>
+      <c r="B206" s="23"/>
     </row>
     <row r="207" ht="15.75" customHeight="1">
-      <c r="B207" s="22"/>
+      <c r="B207" s="23"/>
     </row>
     <row r="208" ht="15.75" customHeight="1">
-      <c r="B208" s="22"/>
+      <c r="B208" s="23"/>
     </row>
     <row r="209" ht="15.75" customHeight="1">
-      <c r="B209" s="22"/>
+      <c r="B209" s="23"/>
     </row>
     <row r="210" ht="15.75" customHeight="1">
-      <c r="B210" s="22"/>
+      <c r="B210" s="23"/>
     </row>
     <row r="211" ht="15.75" customHeight="1">
-      <c r="B211" s="22"/>
+      <c r="B211" s="23"/>
     </row>
     <row r="212" ht="15.75" customHeight="1">
-      <c r="B212" s="22"/>
+      <c r="B212" s="23"/>
     </row>
     <row r="213" ht="15.75" customHeight="1">
-      <c r="B213" s="22"/>
+      <c r="B213" s="23"/>
     </row>
     <row r="214" ht="15.75" customHeight="1">
-      <c r="B214" s="22"/>
+      <c r="B214" s="23"/>
     </row>
     <row r="215" ht="15.75" customHeight="1">
-      <c r="B215" s="22"/>
+      <c r="B215" s="23"/>
     </row>
     <row r="216" ht="15.75" customHeight="1">
-      <c r="B216" s="22"/>
+      <c r="B216" s="23"/>
     </row>
     <row r="217" ht="15.75" customHeight="1">
-      <c r="B217" s="22"/>
+      <c r="B217" s="23"/>
     </row>
     <row r="218" ht="15.75" customHeight="1">
-      <c r="B218" s="22"/>
+      <c r="B218" s="23"/>
     </row>
     <row r="219" ht="15.75" customHeight="1">
-      <c r="B219" s="22"/>
+      <c r="B219" s="23"/>
     </row>
     <row r="220" ht="15.75" customHeight="1">
-      <c r="B220" s="22"/>
+      <c r="B220" s="23"/>
     </row>
     <row r="221" ht="15.75" customHeight="1">
-      <c r="B221" s="22"/>
+      <c r="B221" s="23"/>
     </row>
     <row r="222" ht="15.75" customHeight="1">
-      <c r="B222" s="22"/>
+      <c r="B222" s="23"/>
     </row>
     <row r="223" ht="15.75" customHeight="1">
-      <c r="B223" s="22"/>
+      <c r="B223" s="23"/>
     </row>
     <row r="224" ht="15.75" customHeight="1">
-      <c r="B224" s="22"/>
+      <c r="B224" s="23"/>
     </row>
     <row r="225" ht="15.75" customHeight="1">
-      <c r="B225" s="22"/>
+      <c r="B225" s="23"/>
     </row>
     <row r="226" ht="15.75" customHeight="1">
-      <c r="B226" s="22"/>
+      <c r="B226" s="23"/>
     </row>
     <row r="227" ht="15.75" customHeight="1">
-      <c r="B227" s="22"/>
+      <c r="B227" s="23"/>
     </row>
     <row r="228" ht="15.75" customHeight="1">
-      <c r="B228" s="22"/>
+      <c r="B228" s="23"/>
     </row>
     <row r="229" ht="15.75" customHeight="1">
-      <c r="B229" s="22"/>
+      <c r="B229" s="23"/>
     </row>
     <row r="230" ht="15.75" customHeight="1">
-      <c r="B230" s="22"/>
+      <c r="B230" s="23"/>
     </row>
     <row r="231" ht="15.75" customHeight="1">
-      <c r="B231" s="22"/>
+      <c r="B231" s="23"/>
     </row>
     <row r="232" ht="15.75" customHeight="1">
-      <c r="B232" s="22"/>
+      <c r="B232" s="23"/>
     </row>
     <row r="233" ht="15.75" customHeight="1">
-      <c r="B233" s="22"/>
+      <c r="B233" s="23"/>
     </row>
     <row r="234" ht="15.75" customHeight="1">
-      <c r="B234" s="22"/>
+      <c r="B234" s="23"/>
     </row>
     <row r="235" ht="15.75" customHeight="1">
-      <c r="B235" s="22"/>
+      <c r="B235" s="23"/>
     </row>
     <row r="236" ht="15.75" customHeight="1">
-      <c r="B236" s="22"/>
+      <c r="B236" s="23"/>
     </row>
     <row r="237" ht="15.75" customHeight="1">
-      <c r="B237" s="22"/>
+      <c r="B237" s="23"/>
     </row>
     <row r="238" ht="15.75" customHeight="1">
-      <c r="B238" s="22"/>
+      <c r="B238" s="23"/>
     </row>
     <row r="239" ht="15.75" customHeight="1">
-      <c r="B239" s="22"/>
+      <c r="B239" s="23"/>
     </row>
     <row r="240" ht="15.75" customHeight="1">
-      <c r="B240" s="22"/>
+      <c r="B240" s="23"/>
     </row>
     <row r="241" ht="15.75" customHeight="1">
-      <c r="B241" s="22"/>
+      <c r="B241" s="23"/>
     </row>
     <row r="242" ht="15.75" customHeight="1">
-      <c r="B242" s="22"/>
+      <c r="B242" s="23"/>
     </row>
     <row r="243" ht="15.75" customHeight="1">
-      <c r="B243" s="22"/>
+      <c r="B243" s="23"/>
     </row>
     <row r="244" ht="15.75" customHeight="1">
-      <c r="B244" s="22"/>
+      <c r="B244" s="23"/>
     </row>
     <row r="245" ht="15.75" customHeight="1">
-      <c r="B245" s="22"/>
+      <c r="B245" s="23"/>
     </row>
     <row r="246" ht="15.75" customHeight="1">
-      <c r="B246" s="22"/>
+      <c r="B246" s="23"/>
     </row>
     <row r="247" ht="15.75" customHeight="1">
-      <c r="B247" s="22"/>
+      <c r="B247" s="23"/>
     </row>
     <row r="248" ht="15.75" customHeight="1">
-      <c r="B248" s="22"/>
+      <c r="B248" s="23"/>
     </row>
     <row r="249" ht="15.75" customHeight="1">
-      <c r="B249" s="22"/>
+      <c r="B249" s="23"/>
     </row>
     <row r="250" ht="15.75" customHeight="1">
-      <c r="B250" s="22"/>
+      <c r="B250" s="23"/>
     </row>
     <row r="251" ht="15.75" customHeight="1">
-      <c r="B251" s="22"/>
+      <c r="B251" s="23"/>
     </row>
     <row r="252" ht="15.75" customHeight="1">
-      <c r="B252" s="22"/>
+      <c r="B252" s="23"/>
     </row>
     <row r="253" ht="15.75" customHeight="1">
-      <c r="B253" s="22"/>
+      <c r="B253" s="23"/>
     </row>
     <row r="254" ht="15.75" customHeight="1">
-      <c r="B254" s="22"/>
+      <c r="B254" s="23"/>
     </row>
     <row r="255" ht="15.75" customHeight="1">
-      <c r="B255" s="22"/>
+      <c r="B255" s="23"/>
     </row>
     <row r="256" ht="15.75" customHeight="1">
-      <c r="B256" s="22"/>
+      <c r="B256" s="23"/>
     </row>
     <row r="257" ht="15.75" customHeight="1">
-      <c r="B257" s="22"/>
+      <c r="B257" s="23"/>
     </row>
     <row r="258" ht="15.75" customHeight="1">
-      <c r="B258" s="22"/>
+      <c r="B258" s="23"/>
     </row>
     <row r="259" ht="15.75" customHeight="1">
-      <c r="B259" s="22"/>
+      <c r="B259" s="23"/>
     </row>
     <row r="260" ht="15.75" customHeight="1">
-      <c r="B260" s="22"/>
+      <c r="B260" s="23"/>
     </row>
     <row r="261" ht="15.75" customHeight="1">
-      <c r="B261" s="22"/>
+      <c r="B261" s="23"/>
     </row>
     <row r="262" ht="15.75" customHeight="1">
-      <c r="B262" s="22"/>
+      <c r="B262" s="23"/>
     </row>
     <row r="263" ht="15.75" customHeight="1">
-      <c r="B263" s="22"/>
+      <c r="B263" s="23"/>
     </row>
     <row r="264" ht="15.75" customHeight="1">
-      <c r="B264" s="22"/>
+      <c r="B264" s="23"/>
     </row>
     <row r="265" ht="15.75" customHeight="1">
-      <c r="B265" s="22"/>
+      <c r="B265" s="23"/>
     </row>
     <row r="266" ht="15.75" customHeight="1">
-      <c r="B266" s="22"/>
+      <c r="B266" s="23"/>
     </row>
     <row r="267" ht="15.75" customHeight="1">
-      <c r="B267" s="22"/>
+      <c r="B267" s="23"/>
     </row>
     <row r="268" ht="15.75" customHeight="1">
-      <c r="B268" s="22"/>
+      <c r="B268" s="23"/>
     </row>
     <row r="269" ht="15.75" customHeight="1">
-      <c r="B269" s="22"/>
+      <c r="B269" s="23"/>
     </row>
     <row r="270" ht="15.75" customHeight="1">
-      <c r="B270" s="22"/>
+      <c r="B270" s="23"/>
     </row>
     <row r="271" ht="15.75" customHeight="1">
-      <c r="B271" s="22"/>
+      <c r="B271" s="23"/>
     </row>
     <row r="272" ht="15.75" customHeight="1">
-      <c r="B272" s="22"/>
+      <c r="B272" s="23"/>
     </row>
     <row r="273" ht="15.75" customHeight="1">
-      <c r="B273" s="22"/>
+      <c r="B273" s="23"/>
     </row>
     <row r="274" ht="15.75" customHeight="1">
-      <c r="B274" s="22"/>
+      <c r="B274" s="23"/>
     </row>
     <row r="275" ht="15.75" customHeight="1">
-      <c r="B275" s="22"/>
+      <c r="B275" s="23"/>
     </row>
     <row r="276" ht="15.75" customHeight="1">
-      <c r="B276" s="22"/>
+      <c r="B276" s="23"/>
     </row>
     <row r="277" ht="15.75" customHeight="1">
-      <c r="B277" s="22"/>
+      <c r="B277" s="23"/>
     </row>
     <row r="278" ht="15.75" customHeight="1">
-      <c r="B278" s="22"/>
+      <c r="B278" s="23"/>
     </row>
     <row r="279" ht="15.75" customHeight="1">
-      <c r="B279" s="22"/>
+      <c r="B279" s="23"/>
     </row>
     <row r="280" ht="15.75" customHeight="1">
-      <c r="B280" s="22"/>
+      <c r="B280" s="23"/>
     </row>
     <row r="281" ht="15.75" customHeight="1">
-      <c r="B281" s="22"/>
+      <c r="B281" s="23"/>
     </row>
     <row r="282" ht="15.75" customHeight="1">
-      <c r="B282" s="22"/>
+      <c r="B282" s="23"/>
     </row>
     <row r="283" ht="15.75" customHeight="1">
-      <c r="B283" s="22"/>
+      <c r="B283" s="23"/>
     </row>
     <row r="284" ht="15.75" customHeight="1">
-      <c r="B284" s="22"/>
+      <c r="B284" s="23"/>
     </row>
     <row r="285" ht="15.75" customHeight="1">
-      <c r="B285" s="22"/>
+      <c r="B285" s="23"/>
     </row>
     <row r="286" ht="15.75" customHeight="1">
-      <c r="B286" s="22"/>
+      <c r="B286" s="23"/>
     </row>
     <row r="287" ht="15.75" customHeight="1">
-      <c r="B287" s="22"/>
+      <c r="B287" s="23"/>
     </row>
     <row r="288" ht="15.75" customHeight="1">
-      <c r="B288" s="22"/>
+      <c r="B288" s="23"/>
     </row>
     <row r="289" ht="15.75" customHeight="1">
-      <c r="B289" s="22"/>
+      <c r="B289" s="23"/>
     </row>
     <row r="290" ht="15.75" customHeight="1">
-      <c r="B290" s="22"/>
+      <c r="B290" s="23"/>
     </row>
     <row r="291" ht="15.75" customHeight="1">
-      <c r="B291" s="22"/>
+      <c r="B291" s="23"/>
     </row>
     <row r="292" ht="15.75" customHeight="1">
-      <c r="B292" s="22"/>
+      <c r="B292" s="23"/>
     </row>
     <row r="293" ht="15.75" customHeight="1">
-      <c r="B293" s="22"/>
+      <c r="B293" s="23"/>
     </row>
     <row r="294" ht="15.75" customHeight="1">
-      <c r="B294" s="22"/>
+      <c r="B294" s="23"/>
     </row>
     <row r="295" ht="15.75" customHeight="1">
-      <c r="B295" s="22"/>
+      <c r="B295" s="23"/>
     </row>
     <row r="296" ht="15.75" customHeight="1">
-      <c r="B296" s="22"/>
+      <c r="B296" s="23"/>
     </row>
     <row r="297" ht="15.75" customHeight="1">
-      <c r="B297" s="22"/>
+      <c r="B297" s="23"/>
     </row>
     <row r="298" ht="15.75" customHeight="1">
-      <c r="B298" s="22"/>
+      <c r="B298" s="23"/>
     </row>
     <row r="299" ht="15.75" customHeight="1">
-      <c r="B299" s="22"/>
+      <c r="B299" s="23"/>
     </row>
     <row r="300" ht="15.75" customHeight="1">
-      <c r="B300" s="22"/>
+      <c r="B300" s="23"/>
     </row>
     <row r="301" ht="15.75" customHeight="1">
-      <c r="B301" s="22"/>
+      <c r="B301" s="23"/>
     </row>
     <row r="302" ht="15.75" customHeight="1">
-      <c r="B302" s="22"/>
+      <c r="B302" s="23"/>
     </row>
     <row r="303" ht="15.75" customHeight="1">
-      <c r="B303" s="22"/>
+      <c r="B303" s="23"/>
     </row>
     <row r="304" ht="15.75" customHeight="1">
-      <c r="B304" s="22"/>
+      <c r="B304" s="23"/>
     </row>
     <row r="305" ht="15.75" customHeight="1">
-      <c r="B305" s="22"/>
+      <c r="B305" s="23"/>
     </row>
     <row r="306" ht="15.75" customHeight="1">
-      <c r="B306" s="22"/>
+      <c r="B306" s="23"/>
     </row>
     <row r="307" ht="15.75" customHeight="1">
-      <c r="B307" s="22"/>
+      <c r="B307" s="23"/>
     </row>
     <row r="308" ht="15.75" customHeight="1">
-      <c r="B308" s="22"/>
+      <c r="B308" s="23"/>
     </row>
     <row r="309" ht="15.75" customHeight="1">
-      <c r="B309" s="22"/>
+      <c r="B309" s="23"/>
     </row>
     <row r="310" ht="15.75" customHeight="1">
-      <c r="B310" s="22"/>
+      <c r="B310" s="23"/>
     </row>
     <row r="311" ht="15.75" customHeight="1">
-      <c r="B311" s="22"/>
+      <c r="B311" s="23"/>
     </row>
     <row r="312" ht="15.75" customHeight="1">
-      <c r="B312" s="22"/>
+      <c r="B312" s="23"/>
     </row>
     <row r="313" ht="15.75" customHeight="1">
-      <c r="B313" s="22"/>
+      <c r="B313" s="23"/>
     </row>
     <row r="314" ht="15.75" customHeight="1">
-      <c r="B314" s="22"/>
+      <c r="B314" s="23"/>
     </row>
     <row r="315" ht="15.75" customHeight="1">
-      <c r="B315" s="22"/>
+      <c r="B315" s="23"/>
     </row>
     <row r="316" ht="15.75" customHeight="1">
-      <c r="B316" s="22"/>
+      <c r="B316" s="23"/>
     </row>
     <row r="317" ht="15.75" customHeight="1">
-      <c r="B317" s="22"/>
+      <c r="B317" s="23"/>
     </row>
     <row r="318" ht="15.75" customHeight="1">
-      <c r="B318" s="22"/>
+      <c r="B318" s="23"/>
     </row>
     <row r="319" ht="15.75" customHeight="1">
-      <c r="B319" s="22"/>
+      <c r="B319" s="23"/>
     </row>
     <row r="320" ht="15.75" customHeight="1">
-      <c r="B320" s="22"/>
+      <c r="B320" s="23"/>
     </row>
     <row r="321" ht="15.75" customHeight="1">
-      <c r="B321" s="22"/>
+      <c r="B321" s="23"/>
     </row>
     <row r="322" ht="15.75" customHeight="1">
-      <c r="B322" s="22"/>
+      <c r="B322" s="23"/>
     </row>
     <row r="323" ht="15.75" customHeight="1">
-      <c r="B323" s="22"/>
+      <c r="B323" s="23"/>
     </row>
     <row r="324" ht="15.75" customHeight="1">
-      <c r="B324" s="22"/>
+      <c r="B324" s="23"/>
     </row>
     <row r="325" ht="15.75" customHeight="1">
-      <c r="B325" s="22"/>
+      <c r="B325" s="23"/>
     </row>
     <row r="326" ht="15.75" customHeight="1">
-      <c r="B326" s="22"/>
+      <c r="B326" s="23"/>
     </row>
     <row r="327" ht="15.75" customHeight="1">
-      <c r="B327" s="22"/>
+      <c r="B327" s="23"/>
     </row>
     <row r="328" ht="15.75" customHeight="1">
-      <c r="B328" s="22"/>
+      <c r="B328" s="23"/>
     </row>
     <row r="329" ht="15.75" customHeight="1">
-      <c r="B329" s="22"/>
+      <c r="B329" s="23"/>
     </row>
     <row r="330" ht="15.75" customHeight="1">
-      <c r="B330" s="22"/>
+      <c r="B330" s="23"/>
     </row>
     <row r="331" ht="15.75" customHeight="1">
-      <c r="B331" s="22"/>
+      <c r="B331" s="23"/>
     </row>
     <row r="332" ht="15.75" customHeight="1">
-      <c r="B332" s="22"/>
+      <c r="B332" s="23"/>
     </row>
     <row r="333" ht="15.75" customHeight="1">
-      <c r="B333" s="22"/>
+      <c r="B333" s="23"/>
     </row>
     <row r="334" ht="15.75" customHeight="1">
-      <c r="B334" s="22"/>
+      <c r="B334" s="23"/>
     </row>
     <row r="335" ht="15.75" customHeight="1">
-      <c r="B335" s="22"/>
+      <c r="B335" s="23"/>
     </row>
     <row r="336" ht="15.75" customHeight="1">
-      <c r="B336" s="22"/>
+      <c r="B336" s="23"/>
     </row>
     <row r="337" ht="15.75" customHeight="1">
-      <c r="B337" s="22"/>
+      <c r="B337" s="23"/>
     </row>
     <row r="338" ht="15.75" customHeight="1">
-      <c r="B338" s="22"/>
+      <c r="B338" s="23"/>
     </row>
     <row r="339" ht="15.75" customHeight="1">
-      <c r="B339" s="22"/>
+      <c r="B339" s="23"/>
     </row>
     <row r="340" ht="15.75" customHeight="1">
-      <c r="B340" s="22"/>
+      <c r="B340" s="23"/>
     </row>
     <row r="341" ht="15.75" customHeight="1">
-      <c r="B341" s="22"/>
+      <c r="B341" s="23"/>
     </row>
     <row r="342" ht="15.75" customHeight="1">
-      <c r="B342" s="22"/>
+      <c r="B342" s="23"/>
     </row>
     <row r="343" ht="15.75" customHeight="1">
-      <c r="B343" s="22"/>
+      <c r="B343" s="23"/>
     </row>
     <row r="344" ht="15.75" customHeight="1">
-      <c r="B344" s="22"/>
+      <c r="B344" s="23"/>
     </row>
     <row r="345" ht="15.75" customHeight="1">
-      <c r="B345" s="22"/>
+      <c r="B345" s="23"/>
     </row>
     <row r="346" ht="15.75" customHeight="1">
-      <c r="B346" s="22"/>
+      <c r="B346" s="23"/>
     </row>
     <row r="347" ht="15.75" customHeight="1">
-      <c r="B347" s="22"/>
+      <c r="B347" s="23"/>
     </row>
     <row r="348" ht="15.75" customHeight="1">
-      <c r="B348" s="22"/>
+      <c r="B348" s="23"/>
     </row>
     <row r="349" ht="15.75" customHeight="1">
-      <c r="B349" s="22"/>
+      <c r="B349" s="23"/>
     </row>
     <row r="350" ht="15.75" customHeight="1">
-      <c r="B350" s="22"/>
+      <c r="B350" s="23"/>
     </row>
     <row r="351" ht="15.75" customHeight="1">
-      <c r="B351" s="22"/>
+      <c r="B351" s="23"/>
     </row>
     <row r="352" ht="15.75" customHeight="1">
-      <c r="B352" s="22"/>
+      <c r="B352" s="23"/>
     </row>
     <row r="353" ht="15.75" customHeight="1">
-      <c r="B353" s="22"/>
+      <c r="B353" s="23"/>
     </row>
     <row r="354" ht="15.75" customHeight="1">
-      <c r="B354" s="22"/>
+      <c r="B354" s="23"/>
     </row>
     <row r="355" ht="15.75" customHeight="1">
-      <c r="B355" s="22"/>
+      <c r="B355" s="23"/>
     </row>
     <row r="356" ht="15.75" customHeight="1">
-      <c r="B356" s="22"/>
+      <c r="B356" s="23"/>
     </row>
     <row r="357" ht="15.75" customHeight="1">
-      <c r="B357" s="22"/>
+      <c r="B357" s="23"/>
     </row>
     <row r="358" ht="15.75" customHeight="1">
-      <c r="B358" s="22"/>
+      <c r="B358" s="23"/>
     </row>
     <row r="359" ht="15.75" customHeight="1">
-      <c r="B359" s="22"/>
+      <c r="B359" s="23"/>
     </row>
     <row r="360" ht="15.75" customHeight="1">
-      <c r="B360" s="22"/>
+      <c r="B360" s="23"/>
     </row>
     <row r="361" ht="15.75" customHeight="1">
-      <c r="B361" s="22"/>
+      <c r="B361" s="23"/>
     </row>
     <row r="362" ht="15.75" customHeight="1">
-      <c r="B362" s="22"/>
+      <c r="B362" s="23"/>
     </row>
     <row r="363" ht="15.75" customHeight="1">
-      <c r="B363" s="22"/>
+      <c r="B363" s="23"/>
     </row>
     <row r="364" ht="15.75" customHeight="1">
-      <c r="B364" s="22"/>
+      <c r="B364" s="23"/>
     </row>
     <row r="365" ht="15.75" customHeight="1">
-      <c r="B365" s="22"/>
+      <c r="B365" s="23"/>
     </row>
     <row r="366" ht="15.75" customHeight="1">
-      <c r="B366" s="22"/>
+      <c r="B366" s="23"/>
     </row>
     <row r="367" ht="15.75" customHeight="1">
-      <c r="B367" s="22"/>
+      <c r="B367" s="23"/>
     </row>
     <row r="368" ht="15.75" customHeight="1">
-      <c r="B368" s="22"/>
+      <c r="B368" s="23"/>
     </row>
     <row r="369" ht="15.75" customHeight="1">
-      <c r="B369" s="22"/>
+      <c r="B369" s="23"/>
     </row>
     <row r="370" ht="15.75" customHeight="1">
-      <c r="B370" s="22"/>
+      <c r="B370" s="23"/>
     </row>
     <row r="371" ht="15.75" customHeight="1">
-      <c r="B371" s="22"/>
+      <c r="B371" s="23"/>
     </row>
     <row r="372" ht="15.75" customHeight="1">
-      <c r="B372" s="22"/>
+      <c r="B372" s="23"/>
     </row>
     <row r="373" ht="15.75" customHeight="1">
-      <c r="B373" s="22"/>
+      <c r="B373" s="23"/>
     </row>
     <row r="374" ht="15.75" customHeight="1">
-      <c r="B374" s="22"/>
+      <c r="B374" s="23"/>
     </row>
     <row r="375" ht="15.75" customHeight="1">
-      <c r="B375" s="22"/>
+      <c r="B375" s="23"/>
     </row>
     <row r="376" ht="15.75" customHeight="1">
-      <c r="B376" s="22"/>
+      <c r="B376" s="23"/>
     </row>
     <row r="377" ht="15.75" customHeight="1">
-      <c r="B377" s="22"/>
+      <c r="B377" s="23"/>
     </row>
     <row r="378" ht="15.75" customHeight="1">
-      <c r="B378" s="22"/>
+      <c r="B378" s="23"/>
     </row>
     <row r="379" ht="15.75" customHeight="1">
-      <c r="B379" s="22"/>
+      <c r="B379" s="23"/>
     </row>
     <row r="380" ht="15.75" customHeight="1">
-      <c r="B380" s="22"/>
+      <c r="B380" s="23"/>
     </row>
     <row r="381" ht="15.75" customHeight="1">
-      <c r="B381" s="22"/>
+      <c r="B381" s="23"/>
     </row>
     <row r="382" ht="15.75" customHeight="1">
-      <c r="B382" s="22"/>
+      <c r="B382" s="23"/>
     </row>
     <row r="383" ht="15.75" customHeight="1">
-      <c r="B383" s="22"/>
+      <c r="B383" s="23"/>
     </row>
     <row r="384" ht="15.75" customHeight="1">
-      <c r="B384" s="22"/>
+      <c r="B384" s="23"/>
     </row>
     <row r="385" ht="15.75" customHeight="1">
-      <c r="B385" s="22"/>
+      <c r="B385" s="23"/>
     </row>
     <row r="386" ht="15.75" customHeight="1">
-      <c r="B386" s="22"/>
+      <c r="B386" s="23"/>
     </row>
     <row r="387" ht="15.75" customHeight="1">
-      <c r="B387" s="22"/>
+      <c r="B387" s="23"/>
     </row>
     <row r="388" ht="15.75" customHeight="1">
-      <c r="B388" s="22"/>
+      <c r="B388" s="23"/>
     </row>
     <row r="389" ht="15.75" customHeight="1">
-      <c r="B389" s="22"/>
+      <c r="B389" s="23"/>
     </row>
     <row r="390" ht="15.75" customHeight="1">
-      <c r="B390" s="22"/>
+      <c r="B390" s="23"/>
     </row>
     <row r="391" ht="15.75" customHeight="1">
-      <c r="B391" s="22"/>
+      <c r="B391" s="23"/>
     </row>
     <row r="392" ht="15.75" customHeight="1">
-      <c r="B392" s="22"/>
+      <c r="B392" s="23"/>
     </row>
     <row r="393" ht="15.75" customHeight="1">
-      <c r="B393" s="22"/>
+      <c r="B393" s="23"/>
     </row>
     <row r="394" ht="15.75" customHeight="1">
-      <c r="B394" s="22"/>
+      <c r="B394" s="23"/>
     </row>
     <row r="395" ht="15.75" customHeight="1">
-      <c r="B395" s="22"/>
+      <c r="B395" s="23"/>
     </row>
     <row r="396" ht="15.75" customHeight="1">
-      <c r="B396" s="22"/>
+      <c r="B396" s="23"/>
     </row>
     <row r="397" ht="15.75" customHeight="1">
-      <c r="B397" s="22"/>
+      <c r="B397" s="23"/>
     </row>
     <row r="398" ht="15.75" customHeight="1">
-      <c r="B398" s="22"/>
+      <c r="B398" s="23"/>
     </row>
     <row r="399" ht="15.75" customHeight="1">
-      <c r="B399" s="22"/>
+      <c r="B399" s="23"/>
     </row>
     <row r="400" ht="15.75" customHeight="1">
-      <c r="B400" s="22"/>
+      <c r="B400" s="23"/>
     </row>
     <row r="401" ht="15.75" customHeight="1">
-      <c r="B401" s="22"/>
+      <c r="B401" s="23"/>
     </row>
     <row r="402" ht="15.75" customHeight="1">
-      <c r="B402" s="22"/>
+      <c r="B402" s="23"/>
     </row>
     <row r="403" ht="15.75" customHeight="1">
-      <c r="B403" s="22"/>
+      <c r="B403" s="23"/>
     </row>
     <row r="404" ht="15.75" customHeight="1">
-      <c r="B404" s="22"/>
+      <c r="B404" s="23"/>
     </row>
     <row r="405" ht="15.75" customHeight="1">
-      <c r="B405" s="22"/>
+      <c r="B405" s="23"/>
     </row>
     <row r="406" ht="15.75" customHeight="1">
-      <c r="B406" s="22"/>
+      <c r="B406" s="23"/>
     </row>
     <row r="407" ht="15.75" customHeight="1">
-      <c r="B407" s="22"/>
+      <c r="B407" s="23"/>
     </row>
     <row r="408" ht="15.75" customHeight="1">
-      <c r="B408" s="22"/>
+      <c r="B408" s="23"/>
     </row>
     <row r="409" ht="15.75" customHeight="1">
-      <c r="B409" s="22"/>
+      <c r="B409" s="23"/>
     </row>
     <row r="410" ht="15.75" customHeight="1">
-      <c r="B410" s="22"/>
+      <c r="B410" s="23"/>
     </row>
     <row r="411" ht="15.75" customHeight="1">
-      <c r="B411" s="22"/>
+      <c r="B411" s="23"/>
     </row>
     <row r="412" ht="15.75" customHeight="1">
-      <c r="B412" s="22"/>
+      <c r="B412" s="23"/>
     </row>
     <row r="413" ht="15.75" customHeight="1">
-      <c r="B413" s="22"/>
+      <c r="B413" s="23"/>
     </row>
     <row r="414" ht="15.75" customHeight="1">
-      <c r="B414" s="22"/>
+      <c r="B414" s="23"/>
     </row>
     <row r="415" ht="15.75" customHeight="1">
-      <c r="B415" s="22"/>
+      <c r="B415" s="23"/>
     </row>
     <row r="416" ht="15.75" customHeight="1">
-      <c r="B416" s="22"/>
+      <c r="B416" s="23"/>
     </row>
     <row r="417" ht="15.75" customHeight="1">
-      <c r="B417" s="22"/>
+      <c r="B417" s="23"/>
     </row>
     <row r="418" ht="15.75" customHeight="1">
-      <c r="B418" s="22"/>
+      <c r="B418" s="23"/>
     </row>
     <row r="419" ht="15.75" customHeight="1">
-      <c r="B419" s="22"/>
+      <c r="B419" s="23"/>
     </row>
     <row r="420" ht="15.75" customHeight="1">
-      <c r="B420" s="22"/>
+      <c r="B420" s="23"/>
     </row>
     <row r="421" ht="15.75" customHeight="1">
-      <c r="B421" s="22"/>
+      <c r="B421" s="23"/>
     </row>
     <row r="422" ht="15.75" customHeight="1">
-      <c r="B422" s="22"/>
+      <c r="B422" s="23"/>
     </row>
     <row r="423" ht="15.75" customHeight="1">
-      <c r="B423" s="22"/>
+      <c r="B423" s="23"/>
     </row>
     <row r="424" ht="15.75" customHeight="1">
-      <c r="B424" s="22"/>
+      <c r="B424" s="23"/>
     </row>
     <row r="425" ht="15.75" customHeight="1">
-      <c r="B425" s="22"/>
+      <c r="B425" s="23"/>
     </row>
     <row r="426" ht="15.75" customHeight="1">
-      <c r="B426" s="22"/>
+      <c r="B426" s="23"/>
     </row>
     <row r="427" ht="15.75" customHeight="1">
-      <c r="B427" s="22"/>
+      <c r="B427" s="23"/>
     </row>
     <row r="428" ht="15.75" customHeight="1">
-      <c r="B428" s="22"/>
+      <c r="B428" s="23"/>
     </row>
     <row r="429" ht="15.75" customHeight="1">
-      <c r="B429" s="22"/>
+      <c r="B429" s="23"/>
     </row>
     <row r="430" ht="15.75" customHeight="1">
-      <c r="B430" s="22"/>
+      <c r="B430" s="23"/>
     </row>
     <row r="431" ht="15.75" customHeight="1">
-      <c r="B431" s="22"/>
+      <c r="B431" s="23"/>
     </row>
     <row r="432" ht="15.75" customHeight="1">
-      <c r="B432" s="22"/>
+      <c r="B432" s="23"/>
     </row>
     <row r="433" ht="15.75" customHeight="1">
-      <c r="B433" s="22"/>
+      <c r="B433" s="23"/>
     </row>
     <row r="434" ht="15.75" customHeight="1">
-      <c r="B434" s="22"/>
+      <c r="B434" s="23"/>
     </row>
     <row r="435" ht="15.75" customHeight="1">
-      <c r="B435" s="22"/>
+      <c r="B435" s="23"/>
     </row>
     <row r="436" ht="15.75" customHeight="1">
-      <c r="B436" s="22"/>
+      <c r="B436" s="23"/>
     </row>
     <row r="437" ht="15.75" customHeight="1">
-      <c r="B437" s="22"/>
+      <c r="B437" s="23"/>
     </row>
     <row r="438" ht="15.75" customHeight="1">
-      <c r="B438" s="22"/>
+      <c r="B438" s="23"/>
     </row>
     <row r="439" ht="15.75" customHeight="1">
-      <c r="B439" s="22"/>
+      <c r="B439" s="23"/>
     </row>
     <row r="440" ht="15.75" customHeight="1">
-      <c r="B440" s="22"/>
+      <c r="B440" s="23"/>
     </row>
     <row r="441" ht="15.75" customHeight="1">
-      <c r="B441" s="22"/>
+      <c r="B441" s="23"/>
     </row>
     <row r="442" ht="15.75" customHeight="1">
-      <c r="B442" s="22"/>
+      <c r="B442" s="23"/>
     </row>
     <row r="443" ht="15.75" customHeight="1">
-      <c r="B443" s="22"/>
+      <c r="B443" s="23"/>
     </row>
     <row r="444" ht="15.75" customHeight="1">
-      <c r="B444" s="22"/>
+      <c r="B444" s="23"/>
     </row>
     <row r="445" ht="15.75" customHeight="1">
-      <c r="B445" s="22"/>
+      <c r="B445" s="23"/>
     </row>
     <row r="446" ht="15.75" customHeight="1">
-      <c r="B446" s="22"/>
+      <c r="B446" s="23"/>
     </row>
     <row r="447" ht="15.75" customHeight="1">
-      <c r="B447" s="22"/>
+      <c r="B447" s="23"/>
     </row>
     <row r="448" ht="15.75" customHeight="1">
-      <c r="B448" s="22"/>
+      <c r="B448" s="23"/>
     </row>
     <row r="449" ht="15.75" customHeight="1">
-      <c r="B449" s="22"/>
+      <c r="B449" s="23"/>
     </row>
     <row r="450" ht="15.75" customHeight="1">
-      <c r="B450" s="22"/>
+      <c r="B450" s="23"/>
     </row>
     <row r="451" ht="15.75" customHeight="1">
-      <c r="B451" s="22"/>
+      <c r="B451" s="23"/>
     </row>
     <row r="452" ht="15.75" customHeight="1">
-      <c r="B452" s="22"/>
+      <c r="B452" s="23"/>
     </row>
     <row r="453" ht="15.75" customHeight="1">
-      <c r="B453" s="22"/>
+      <c r="B453" s="23"/>
     </row>
     <row r="454" ht="15.75" customHeight="1">
-      <c r="B454" s="22"/>
+      <c r="B454" s="23"/>
     </row>
     <row r="455" ht="15.75" customHeight="1">
-      <c r="B455" s="22"/>
+      <c r="B455" s="23"/>
     </row>
     <row r="456" ht="15.75" customHeight="1">
-      <c r="B456" s="22"/>
+      <c r="B456" s="23"/>
     </row>
     <row r="457" ht="15.75" customHeight="1">
-      <c r="B457" s="22"/>
+      <c r="B457" s="23"/>
     </row>
     <row r="458" ht="15.75" customHeight="1">
-      <c r="B458" s="22"/>
+      <c r="B458" s="23"/>
     </row>
     <row r="459" ht="15.75" customHeight="1">
-      <c r="B459" s="22"/>
+      <c r="B459" s="23"/>
     </row>
     <row r="460" ht="15.75" customHeight="1">
-      <c r="B460" s="22"/>
+      <c r="B460" s="23"/>
     </row>
     <row r="461" ht="15.75" customHeight="1">
-      <c r="B461" s="22"/>
+      <c r="B461" s="23"/>
     </row>
     <row r="462" ht="15.75" customHeight="1">
-      <c r="B462" s="22"/>
+      <c r="B462" s="23"/>
     </row>
     <row r="463" ht="15.75" customHeight="1">
-      <c r="B463" s="22"/>
+      <c r="B463" s="23"/>
     </row>
     <row r="464" ht="15.75" customHeight="1">
-      <c r="B464" s="22"/>
+      <c r="B464" s="23"/>
     </row>
     <row r="465" ht="15.75" customHeight="1">
-      <c r="B465" s="22"/>
+      <c r="B465" s="23"/>
     </row>
     <row r="466" ht="15.75" customHeight="1">
-      <c r="B466" s="22"/>
+      <c r="B466" s="23"/>
     </row>
     <row r="467" ht="15.75" customHeight="1">
-      <c r="B467" s="22"/>
+      <c r="B467" s="23"/>
     </row>
     <row r="468" ht="15.75" customHeight="1">
-      <c r="B468" s="22"/>
+      <c r="B468" s="23"/>
     </row>
     <row r="469" ht="15.75" customHeight="1">
-      <c r="B469" s="22"/>
+      <c r="B469" s="23"/>
     </row>
     <row r="470" ht="15.75" customHeight="1">
-      <c r="B470" s="22"/>
+      <c r="B470" s="23"/>
     </row>
     <row r="471" ht="15.75" customHeight="1">
-      <c r="B471" s="22"/>
+      <c r="B471" s="23"/>
     </row>
     <row r="472" ht="15.75" customHeight="1">
-      <c r="B472" s="22"/>
+      <c r="B472" s="23"/>
     </row>
     <row r="473" ht="15.75" customHeight="1">
-      <c r="B473" s="22"/>
+      <c r="B473" s="23"/>
     </row>
     <row r="474" ht="15.75" customHeight="1">
-      <c r="B474" s="22"/>
+      <c r="B474" s="23"/>
     </row>
     <row r="475" ht="15.75" customHeight="1">
-      <c r="B475" s="22"/>
+      <c r="B475" s="23"/>
     </row>
     <row r="476" ht="15.75" customHeight="1">
-      <c r="B476" s="22"/>
+      <c r="B476" s="23"/>
     </row>
     <row r="477" ht="15.75" customHeight="1">
-      <c r="B477" s="22"/>
+      <c r="B477" s="23"/>
     </row>
     <row r="478" ht="15.75" customHeight="1">
-      <c r="B478" s="22"/>
+      <c r="B478" s="23"/>
     </row>
     <row r="479" ht="15.75" customHeight="1">
-      <c r="B479" s="22"/>
+      <c r="B479" s="23"/>
     </row>
     <row r="480" ht="15.75" customHeight="1">
-      <c r="B480" s="22"/>
+      <c r="B480" s="23"/>
     </row>
     <row r="481" ht="15.75" customHeight="1">
-      <c r="B481" s="22"/>
+      <c r="B481" s="23"/>
     </row>
     <row r="482" ht="15.75" customHeight="1">
-      <c r="B482" s="22"/>
+      <c r="B482" s="23"/>
     </row>
     <row r="483" ht="15.75" customHeight="1">
-      <c r="B483" s="22"/>
+      <c r="B483" s="23"/>
     </row>
     <row r="484" ht="15.75" customHeight="1">
-      <c r="B484" s="22"/>
+      <c r="B484" s="23"/>
     </row>
     <row r="485" ht="15.75" customHeight="1">
-      <c r="B485" s="22"/>
+      <c r="B485" s="23"/>
     </row>
     <row r="486" ht="15.75" customHeight="1">
-      <c r="B486" s="22"/>
+      <c r="B486" s="23"/>
     </row>
     <row r="487" ht="15.75" customHeight="1">
-      <c r="B487" s="22"/>
+      <c r="B487" s="23"/>
     </row>
     <row r="488" ht="15.75" customHeight="1">
-      <c r="B488" s="22"/>
+      <c r="B488" s="23"/>
     </row>
     <row r="489" ht="15.75" customHeight="1">
-      <c r="B489" s="22"/>
+      <c r="B489" s="23"/>
     </row>
     <row r="490" ht="15.75" customHeight="1">
-      <c r="B490" s="22"/>
+      <c r="B490" s="23"/>
     </row>
     <row r="491" ht="15.75" customHeight="1">
-      <c r="B491" s="22"/>
+      <c r="B491" s="23"/>
     </row>
     <row r="492" ht="15.75" customHeight="1">
-      <c r="B492" s="22"/>
+      <c r="B492" s="23"/>
     </row>
     <row r="493" ht="15.75" customHeight="1">
-      <c r="B493" s="22"/>
+      <c r="B493" s="23"/>
     </row>
     <row r="494" ht="15.75" customHeight="1">
-      <c r="B494" s="22"/>
+      <c r="B494" s="23"/>
     </row>
     <row r="495" ht="15.75" customHeight="1">
-      <c r="B495" s="22"/>
+      <c r="B495" s="23"/>
     </row>
     <row r="496" ht="15.75" customHeight="1">
-      <c r="B496" s="22"/>
+      <c r="B496" s="23"/>
     </row>
     <row r="497" ht="15.75" customHeight="1">
-      <c r="B497" s="22"/>
+      <c r="B497" s="23"/>
     </row>
     <row r="498" ht="15.75" customHeight="1">
-      <c r="B498" s="22"/>
+      <c r="B498" s="23"/>
     </row>
     <row r="499" ht="15.75" customHeight="1">
-      <c r="B499" s="22"/>
+      <c r="B499" s="23"/>
     </row>
     <row r="500" ht="15.75" customHeight="1">
-      <c r="B500" s="22"/>
+      <c r="B500" s="23"/>
     </row>
     <row r="501" ht="15.75" customHeight="1">
-      <c r="B501" s="22"/>
+      <c r="B501" s="23"/>
     </row>
     <row r="502" ht="15.75" customHeight="1">
-      <c r="B502" s="22"/>
+      <c r="B502" s="23"/>
     </row>
     <row r="503" ht="15.75" customHeight="1">
-      <c r="B503" s="22"/>
+      <c r="B503" s="23"/>
     </row>
     <row r="504" ht="15.75" customHeight="1">
-      <c r="B504" s="22"/>
+      <c r="B504" s="23"/>
     </row>
     <row r="505" ht="15.75" customHeight="1">
-      <c r="B505" s="22"/>
+      <c r="B505" s="23"/>
     </row>
     <row r="506" ht="15.75" customHeight="1">
-      <c r="B506" s="22"/>
+      <c r="B506" s="23"/>
     </row>
     <row r="507" ht="15.75" customHeight="1">
-      <c r="B507" s="22"/>
+      <c r="B507" s="23"/>
     </row>
     <row r="508" ht="15.75" customHeight="1">
-      <c r="B508" s="22"/>
+      <c r="B508" s="23"/>
     </row>
     <row r="509" ht="15.75" customHeight="1">
-      <c r="B509" s="22"/>
+      <c r="B509" s="23"/>
     </row>
     <row r="510" ht="15.75" customHeight="1">
-      <c r="B510" s="22"/>
+      <c r="B510" s="23"/>
     </row>
     <row r="511" ht="15.75" customHeight="1">
-      <c r="B511" s="22"/>
+      <c r="B511" s="23"/>
     </row>
     <row r="512" ht="15.75" customHeight="1">
-      <c r="B512" s="22"/>
+      <c r="B512" s="23"/>
     </row>
     <row r="513" ht="15.75" customHeight="1">
-      <c r="B513" s="22"/>
+      <c r="B513" s="23"/>
     </row>
     <row r="514" ht="15.75" customHeight="1">
-      <c r="B514" s="22"/>
+      <c r="B514" s="23"/>
     </row>
     <row r="515" ht="15.75" customHeight="1">
-      <c r="B515" s="22"/>
+      <c r="B515" s="23"/>
     </row>
     <row r="516" ht="15.75" customHeight="1">
-      <c r="B516" s="22"/>
+      <c r="B516" s="23"/>
     </row>
     <row r="517" ht="15.75" customHeight="1">
-      <c r="B517" s="22"/>
+      <c r="B517" s="23"/>
     </row>
     <row r="518" ht="15.75" customHeight="1">
-      <c r="B518" s="22"/>
+      <c r="B518" s="23"/>
     </row>
     <row r="519" ht="15.75" customHeight="1">
-      <c r="B519" s="22"/>
+      <c r="B519" s="23"/>
     </row>
     <row r="520" ht="15.75" customHeight="1">
-      <c r="B520" s="22"/>
+      <c r="B520" s="23"/>
     </row>
     <row r="521" ht="15.75" customHeight="1">
-      <c r="B521" s="22"/>
+      <c r="B521" s="23"/>
     </row>
     <row r="522" ht="15.75" customHeight="1">
-      <c r="B522" s="22"/>
+      <c r="B522" s="23"/>
     </row>
     <row r="523" ht="15.75" customHeight="1">
-      <c r="B523" s="22"/>
+      <c r="B523" s="23"/>
     </row>
     <row r="524" ht="15.75" customHeight="1">
-      <c r="B524" s="22"/>
+      <c r="B524" s="23"/>
     </row>
     <row r="525" ht="15.75" customHeight="1">
-      <c r="B525" s="22"/>
+      <c r="B525" s="23"/>
     </row>
     <row r="526" ht="15.75" customHeight="1">
-      <c r="B526" s="22"/>
+      <c r="B526" s="23"/>
     </row>
     <row r="527" ht="15.75" customHeight="1">
-      <c r="B527" s="22"/>
+      <c r="B527" s="23"/>
     </row>
     <row r="528" ht="15.75" customHeight="1">
-      <c r="B528" s="22"/>
+      <c r="B528" s="23"/>
     </row>
     <row r="529" ht="15.75" customHeight="1">
-      <c r="B529" s="22"/>
+      <c r="B529" s="23"/>
     </row>
     <row r="530" ht="15.75" customHeight="1">
-      <c r="B530" s="22"/>
+      <c r="B530" s="23"/>
     </row>
     <row r="531" ht="15.75" customHeight="1">
-      <c r="B531" s="22"/>
+      <c r="B531" s="23"/>
     </row>
     <row r="532" ht="15.75" customHeight="1">
-      <c r="B532" s="22"/>
+      <c r="B532" s="23"/>
     </row>
     <row r="533" ht="15.75" customHeight="1">
-      <c r="B533" s="22"/>
+      <c r="B533" s="23"/>
     </row>
     <row r="534" ht="15.75" customHeight="1">
-      <c r="B534" s="22"/>
+      <c r="B534" s="23"/>
     </row>
     <row r="535" ht="15.75" customHeight="1">
-      <c r="B535" s="22"/>
+      <c r="B535" s="23"/>
     </row>
     <row r="536" ht="15.75" customHeight="1">
-      <c r="B536" s="22"/>
+      <c r="B536" s="23"/>
     </row>
     <row r="537" ht="15.75" customHeight="1">
-      <c r="B537" s="22"/>
+      <c r="B537" s="23"/>
     </row>
     <row r="538" ht="15.75" customHeight="1">
-      <c r="B538" s="22"/>
+      <c r="B538" s="23"/>
     </row>
     <row r="539" ht="15.75" customHeight="1">
-      <c r="B539" s="22"/>
+      <c r="B539" s="23"/>
     </row>
     <row r="540" ht="15.75" customHeight="1">
-      <c r="B540" s="22"/>
+      <c r="B540" s="23"/>
     </row>
     <row r="541" ht="15.75" customHeight="1">
-      <c r="B541" s="22"/>
+      <c r="B541" s="23"/>
     </row>
     <row r="542" ht="15.75" customHeight="1">
-      <c r="B542" s="22"/>
+      <c r="B542" s="23"/>
     </row>
     <row r="543" ht="15.75" customHeight="1">
-      <c r="B543" s="22"/>
+      <c r="B543" s="23"/>
     </row>
     <row r="544" ht="15.75" customHeight="1">
-      <c r="B544" s="22"/>
+      <c r="B544" s="23"/>
     </row>
     <row r="545" ht="15.75" customHeight="1">
-      <c r="B545" s="22"/>
+      <c r="B545" s="23"/>
     </row>
     <row r="546" ht="15.75" customHeight="1">
-      <c r="B546" s="22"/>
+      <c r="B546" s="23"/>
     </row>
     <row r="547" ht="15.75" customHeight="1">
-      <c r="B547" s="22"/>
+      <c r="B547" s="23"/>
     </row>
     <row r="548" ht="15.75" customHeight="1">
-      <c r="B548" s="22"/>
+      <c r="B548" s="23"/>
     </row>
     <row r="549" ht="15.75" customHeight="1">
-      <c r="B549" s="22"/>
+      <c r="B549" s="23"/>
     </row>
     <row r="550" ht="15.75" customHeight="1">
-      <c r="B550" s="22"/>
+      <c r="B550" s="23"/>
     </row>
     <row r="551" ht="15.75" customHeight="1">
-      <c r="B551" s="22"/>
+      <c r="B551" s="23"/>
     </row>
     <row r="552" ht="15.75" customHeight="1">
-      <c r="B552" s="22"/>
+      <c r="B552" s="23"/>
     </row>
     <row r="553" ht="15.75" customHeight="1">
-      <c r="B553" s="22"/>
+      <c r="B553" s="23"/>
     </row>
     <row r="554" ht="15.75" customHeight="1">
-      <c r="B554" s="22"/>
+      <c r="B554" s="23"/>
     </row>
     <row r="555" ht="15.75" customHeight="1">
-      <c r="B555" s="22"/>
+      <c r="B555" s="23"/>
     </row>
     <row r="556" ht="15.75" customHeight="1">
-      <c r="B556" s="22"/>
+      <c r="B556" s="23"/>
     </row>
     <row r="557" ht="15.75" customHeight="1">
-      <c r="B557" s="22"/>
+      <c r="B557" s="23"/>
     </row>
     <row r="558" ht="15.75" customHeight="1">
-      <c r="B558" s="22"/>
+      <c r="B558" s="23"/>
     </row>
     <row r="559" ht="15.75" customHeight="1">
-      <c r="B559" s="22"/>
+      <c r="B559" s="23"/>
     </row>
     <row r="560" ht="15.75" customHeight="1">
-      <c r="B560" s="22"/>
+      <c r="B560" s="23"/>
     </row>
     <row r="561" ht="15.75" customHeight="1">
-      <c r="B561" s="22"/>
+      <c r="B561" s="23"/>
     </row>
     <row r="562" ht="15.75" customHeight="1">
-      <c r="B562" s="22"/>
+      <c r="B562" s="23"/>
     </row>
     <row r="563" ht="15.75" customHeight="1">
-      <c r="B563" s="22"/>
+      <c r="B563" s="23"/>
     </row>
     <row r="564" ht="15.75" customHeight="1">
-      <c r="B564" s="22"/>
+      <c r="B564" s="23"/>
     </row>
     <row r="565" ht="15.75" customHeight="1">
-      <c r="B565" s="22"/>
+      <c r="B565" s="23"/>
     </row>
     <row r="566" ht="15.75" customHeight="1">
-      <c r="B566" s="22"/>
+      <c r="B566" s="23"/>
     </row>
     <row r="567" ht="15.75" customHeight="1">
-      <c r="B567" s="22"/>
+      <c r="B567" s="23"/>
     </row>
     <row r="568" ht="15.75" customHeight="1">
-      <c r="B568" s="22"/>
+      <c r="B568" s="23"/>
     </row>
     <row r="569" ht="15.75" customHeight="1">
-      <c r="B569" s="22"/>
+      <c r="B569" s="23"/>
     </row>
     <row r="570" ht="15.75" customHeight="1">
-      <c r="B570" s="22"/>
+      <c r="B570" s="23"/>
     </row>
     <row r="571" ht="15.75" customHeight="1">
-      <c r="B571" s="22"/>
+      <c r="B571" s="23"/>
     </row>
     <row r="572" ht="15.75" customHeight="1">
-      <c r="B572" s="22"/>
+      <c r="B572" s="23"/>
     </row>
     <row r="573" ht="15.75" customHeight="1">
-      <c r="B573" s="22"/>
+      <c r="B573" s="23"/>
     </row>
     <row r="574" ht="15.75" customHeight="1">
-      <c r="B574" s="22"/>
+      <c r="B574" s="23"/>
     </row>
     <row r="575" ht="15.75" customHeight="1">
-      <c r="B575" s="22"/>
+      <c r="B575" s="23"/>
     </row>
     <row r="576" ht="15.75" customHeight="1">
-      <c r="B576" s="22"/>
+      <c r="B576" s="23"/>
     </row>
     <row r="577" ht="15.75" customHeight="1">
-      <c r="B577" s="22"/>
+      <c r="B577" s="23"/>
     </row>
     <row r="578" ht="15.75" customHeight="1">
-      <c r="B578" s="22"/>
+      <c r="B578" s="23"/>
     </row>
     <row r="579" ht="15.75" customHeight="1">
-      <c r="B579" s="22"/>
+      <c r="B579" s="23"/>
     </row>
     <row r="580" ht="15.75" customHeight="1">
-      <c r="B580" s="22"/>
+      <c r="B580" s="23"/>
     </row>
     <row r="581" ht="15.75" customHeight="1">
-      <c r="B581" s="22"/>
+      <c r="B581" s="23"/>
     </row>
     <row r="582" ht="15.75" customHeight="1">
-      <c r="B582" s="22"/>
+      <c r="B582" s="23"/>
     </row>
     <row r="583" ht="15.75" customHeight="1">
-      <c r="B583" s="22"/>
+      <c r="B583" s="23"/>
     </row>
     <row r="584" ht="15.75" customHeight="1">
-      <c r="B584" s="22"/>
+      <c r="B584" s="23"/>
     </row>
     <row r="585" ht="15.75" customHeight="1">
-      <c r="B585" s="22"/>
+      <c r="B585" s="23"/>
     </row>
     <row r="586" ht="15.75" customHeight="1">
-      <c r="B586" s="22"/>
+      <c r="B586" s="23"/>
     </row>
     <row r="587" ht="15.75" customHeight="1">
-      <c r="B587" s="22"/>
+      <c r="B587" s="23"/>
     </row>
     <row r="588" ht="15.75" customHeight="1">
-      <c r="B588" s="22"/>
+      <c r="B588" s="23"/>
     </row>
     <row r="589" ht="15.75" customHeight="1">
-      <c r="B589" s="22"/>
+      <c r="B589" s="23"/>
     </row>
     <row r="590" ht="15.75" customHeight="1">
-      <c r="B590" s="22"/>
+      <c r="B590" s="23"/>
     </row>
     <row r="591" ht="15.75" customHeight="1">
-      <c r="B591" s="22"/>
+      <c r="B591" s="23"/>
     </row>
     <row r="592" ht="15.75" customHeight="1">
-      <c r="B592" s="22"/>
+      <c r="B592" s="23"/>
     </row>
     <row r="593" ht="15.75" customHeight="1">
-      <c r="B593" s="22"/>
+      <c r="B593" s="23"/>
     </row>
     <row r="594" ht="15.75" customHeight="1">
-      <c r="B594" s="22"/>
+      <c r="B594" s="23"/>
     </row>
     <row r="595" ht="15.75" customHeight="1">
-      <c r="B595" s="22"/>
+      <c r="B595" s="23"/>
     </row>
     <row r="596" ht="15.75" customHeight="1">
-      <c r="B596" s="22"/>
+      <c r="B596" s="23"/>
     </row>
     <row r="597" ht="15.75" customHeight="1">
-      <c r="B597" s="22"/>
+      <c r="B597" s="23"/>
     </row>
     <row r="598" ht="15.75" customHeight="1">
-      <c r="B598" s="22"/>
+      <c r="B598" s="23"/>
     </row>
     <row r="599" ht="15.75" customHeight="1">
-      <c r="B599" s="22"/>
+      <c r="B599" s="23"/>
     </row>
     <row r="600" ht="15.75" customHeight="1">
-      <c r="B600" s="22"/>
+      <c r="B600" s="23"/>
     </row>
     <row r="601" ht="15.75" customHeight="1">
-      <c r="B601" s="22"/>
+      <c r="B601" s="23"/>
     </row>
     <row r="602" ht="15.75" customHeight="1">
-      <c r="B602" s="22"/>
+      <c r="B602" s="23"/>
     </row>
     <row r="603" ht="15.75" customHeight="1">
-      <c r="B603" s="22"/>
+      <c r="B603" s="23"/>
     </row>
     <row r="604" ht="15.75" customHeight="1">
-      <c r="B604" s="22"/>
+      <c r="B604" s="23"/>
     </row>
     <row r="605" ht="15.75" customHeight="1">
-      <c r="B605" s="22"/>
+      <c r="B605" s="23"/>
     </row>
     <row r="606" ht="15.75" customHeight="1">
-      <c r="B606" s="22"/>
+      <c r="B606" s="23"/>
     </row>
     <row r="607" ht="15.75" customHeight="1">
-      <c r="B607" s="22"/>
+      <c r="B607" s="23"/>
     </row>
     <row r="608" ht="15.75" customHeight="1">
-      <c r="B608" s="22"/>
+      <c r="B608" s="23"/>
     </row>
     <row r="609" ht="15.75" customHeight="1">
-      <c r="B609" s="22"/>
+      <c r="B609" s="23"/>
     </row>
     <row r="610" ht="15.75" customHeight="1">
-      <c r="B610" s="22"/>
+      <c r="B610" s="23"/>
     </row>
     <row r="611" ht="15.75" customHeight="1">
-      <c r="B611" s="22"/>
+      <c r="B611" s="23"/>
     </row>
     <row r="612" ht="15.75" customHeight="1">
-      <c r="B612" s="22"/>
+      <c r="B612" s="23"/>
     </row>
     <row r="613" ht="15.75" customHeight="1">
-      <c r="B613" s="22"/>
+      <c r="B613" s="23"/>
     </row>
     <row r="614" ht="15.75" customHeight="1">
-      <c r="B614" s="22"/>
+      <c r="B614" s="23"/>
     </row>
     <row r="615" ht="15.75" customHeight="1">
-      <c r="B615" s="22"/>
+      <c r="B615" s="23"/>
     </row>
     <row r="616" ht="15.75" customHeight="1">
-      <c r="B616" s="22"/>
+      <c r="B616" s="23"/>
     </row>
     <row r="617" ht="15.75" customHeight="1">
-      <c r="B617" s="22"/>
+      <c r="B617" s="23"/>
     </row>
     <row r="618" ht="15.75" customHeight="1">
-      <c r="B618" s="22"/>
+      <c r="B618" s="23"/>
     </row>
     <row r="619" ht="15.75" customHeight="1">
-      <c r="B619" s="22"/>
+      <c r="B619" s="23"/>
     </row>
     <row r="620" ht="15.75" customHeight="1">
-      <c r="B620" s="22"/>
+      <c r="B620" s="23"/>
     </row>
     <row r="621" ht="15.75" customHeight="1">
-      <c r="B621" s="22"/>
+      <c r="B621" s="23"/>
     </row>
     <row r="622" ht="15.75" customHeight="1">
-      <c r="B622" s="22"/>
+      <c r="B622" s="23"/>
     </row>
     <row r="623" ht="15.75" customHeight="1">
-      <c r="B623" s="22"/>
+      <c r="B623" s="23"/>
     </row>
     <row r="624" ht="15.75" customHeight="1">
-      <c r="B624" s="22"/>
+      <c r="B624" s="23"/>
     </row>
     <row r="625" ht="15.75" customHeight="1">
-      <c r="B625" s="22"/>
+      <c r="B625" s="23"/>
     </row>
     <row r="626" ht="15.75" customHeight="1">
-      <c r="B626" s="22"/>
+      <c r="B626" s="23"/>
     </row>
     <row r="627" ht="15.75" customHeight="1">
-      <c r="B627" s="22"/>
+      <c r="B627" s="23"/>
     </row>
     <row r="628" ht="15.75" customHeight="1">
-      <c r="B628" s="22"/>
+      <c r="B628" s="23"/>
     </row>
     <row r="629" ht="15.75" customHeight="1">
-      <c r="B629" s="22"/>
+      <c r="B629" s="23"/>
     </row>
     <row r="630" ht="15.75" customHeight="1">
-      <c r="B630" s="22"/>
+      <c r="B630" s="23"/>
     </row>
     <row r="631" ht="15.75" customHeight="1">
-      <c r="B631" s="22"/>
+      <c r="B631" s="23"/>
     </row>
     <row r="632" ht="15.75" customHeight="1">
-      <c r="B632" s="22"/>
+      <c r="B632" s="23"/>
     </row>
     <row r="633" ht="15.75" customHeight="1">
-      <c r="B633" s="22"/>
+      <c r="B633" s="23"/>
     </row>
     <row r="634" ht="15.75" customHeight="1">
-      <c r="B634" s="22"/>
+      <c r="B634" s="23"/>
     </row>
     <row r="635" ht="15.75" customHeight="1">
-      <c r="B635" s="22"/>
+      <c r="B635" s="23"/>
     </row>
     <row r="636" ht="15.75" customHeight="1">
-      <c r="B636" s="22"/>
+      <c r="B636" s="23"/>
     </row>
     <row r="637" ht="15.75" customHeight="1">
-      <c r="B637" s="22"/>
+      <c r="B637" s="23"/>
     </row>
     <row r="638" ht="15.75" customHeight="1">
-      <c r="B638" s="22"/>
+      <c r="B638" s="23"/>
     </row>
     <row r="639" ht="15.75" customHeight="1">
-      <c r="B639" s="22"/>
+      <c r="B639" s="23"/>
     </row>
     <row r="640" ht="15.75" customHeight="1">
-      <c r="B640" s="22"/>
+      <c r="B640" s="23"/>
     </row>
     <row r="641" ht="15.75" customHeight="1">
-      <c r="B641" s="22"/>
+      <c r="B641" s="23"/>
     </row>
     <row r="642" ht="15.75" customHeight="1">
-      <c r="B642" s="22"/>
+      <c r="B642" s="23"/>
     </row>
     <row r="643" ht="15.75" customHeight="1">
-      <c r="B643" s="22"/>
+      <c r="B643" s="23"/>
     </row>
     <row r="644" ht="15.75" customHeight="1">
-      <c r="B644" s="22"/>
+      <c r="B644" s="23"/>
     </row>
     <row r="645" ht="15.75" customHeight="1">
-      <c r="B645" s="22"/>
+      <c r="B645" s="23"/>
     </row>
     <row r="646" ht="15.75" customHeight="1">
-      <c r="B646" s="22"/>
+      <c r="B646" s="23"/>
     </row>
     <row r="647" ht="15.75" customHeight="1">
-      <c r="B647" s="22"/>
+      <c r="B647" s="23"/>
     </row>
     <row r="648" ht="15.75" customHeight="1">
-      <c r="B648" s="22"/>
+      <c r="B648" s="23"/>
     </row>
     <row r="649" ht="15.75" customHeight="1">
-      <c r="B649" s="22"/>
+      <c r="B649" s="23"/>
     </row>
     <row r="650" ht="15.75" customHeight="1">
-      <c r="B650" s="22"/>
+      <c r="B650" s="23"/>
     </row>
     <row r="651" ht="15.75" customHeight="1">
-      <c r="B651" s="22"/>
+      <c r="B651" s="23"/>
     </row>
     <row r="652" ht="15.75" customHeight="1">
-      <c r="B652" s="22"/>
+      <c r="B652" s="23"/>
     </row>
     <row r="653" ht="15.75" customHeight="1">
-      <c r="B653" s="22"/>
+      <c r="B653" s="23"/>
     </row>
     <row r="654" ht="15.75" customHeight="1">
-      <c r="B654" s="22"/>
+      <c r="B654" s="23"/>
     </row>
     <row r="655" ht="15.75" customHeight="1">
-      <c r="B655" s="22"/>
+      <c r="B655" s="23"/>
     </row>
     <row r="656" ht="15.75" customHeight="1">
-      <c r="B656" s="22"/>
+      <c r="B656" s="23"/>
     </row>
     <row r="657" ht="15.75" customHeight="1">
-      <c r="B657" s="22"/>
+      <c r="B657" s="23"/>
     </row>
     <row r="658" ht="15.75" customHeight="1">
-      <c r="B658" s="22"/>
+      <c r="B658" s="23"/>
     </row>
     <row r="659" ht="15.75" customHeight="1">
-      <c r="B659" s="22"/>
+      <c r="B659" s="23"/>
     </row>
     <row r="660" ht="15.75" customHeight="1">
-      <c r="B660" s="22"/>
+      <c r="B660" s="23"/>
     </row>
     <row r="661" ht="15.75" customHeight="1">
-      <c r="B661" s="22"/>
+      <c r="B661" s="23"/>
     </row>
     <row r="662" ht="15.75" customHeight="1">
-      <c r="B662" s="22"/>
+      <c r="B662" s="23"/>
     </row>
     <row r="663" ht="15.75" customHeight="1">
-      <c r="B663" s="22"/>
+      <c r="B663" s="23"/>
     </row>
     <row r="664" ht="15.75" customHeight="1">
-      <c r="B664" s="22"/>
+      <c r="B664" s="23"/>
     </row>
     <row r="665" ht="15.75" customHeight="1">
-      <c r="B665" s="22"/>
+      <c r="B665" s="23"/>
     </row>
     <row r="666" ht="15.75" customHeight="1">
-      <c r="B666" s="22"/>
+      <c r="B666" s="23"/>
     </row>
     <row r="667" ht="15.75" customHeight="1">
-      <c r="B667" s="22"/>
+      <c r="B667" s="23"/>
     </row>
     <row r="668" ht="15.75" customHeight="1">
-      <c r="B668" s="22"/>
+      <c r="B668" s="23"/>
     </row>
     <row r="669" ht="15.75" customHeight="1">
-      <c r="B669" s="22"/>
+      <c r="B669" s="23"/>
     </row>
     <row r="670" ht="15.75" customHeight="1">
-      <c r="B670" s="22"/>
+      <c r="B670" s="23"/>
     </row>
     <row r="671" ht="15.75" customHeight="1">
-      <c r="B671" s="22"/>
+      <c r="B671" s="23"/>
     </row>
     <row r="672" ht="15.75" customHeight="1">
-      <c r="B672" s="22"/>
+      <c r="B672" s="23"/>
     </row>
     <row r="673" ht="15.75" customHeight="1">
-      <c r="B673" s="22"/>
+      <c r="B673" s="23"/>
     </row>
     <row r="674" ht="15.75" customHeight="1">
-      <c r="B674" s="22"/>
+      <c r="B674" s="23"/>
     </row>
     <row r="675" ht="15.75" customHeight="1">
-      <c r="B675" s="22"/>
+      <c r="B675" s="23"/>
     </row>
     <row r="676" ht="15.75" customHeight="1">
-      <c r="B676" s="22"/>
+      <c r="B676" s="23"/>
     </row>
     <row r="677" ht="15.75" customHeight="1">
-      <c r="B677" s="22"/>
+      <c r="B677" s="23"/>
     </row>
     <row r="678" ht="15.75" customHeight="1">
-      <c r="B678" s="22"/>
+      <c r="B678" s="23"/>
     </row>
     <row r="679" ht="15.75" customHeight="1">
-      <c r="B679" s="22"/>
+      <c r="B679" s="23"/>
     </row>
     <row r="680" ht="15.75" customHeight="1">
-      <c r="B680" s="22"/>
+      <c r="B680" s="23"/>
     </row>
     <row r="681" ht="15.75" customHeight="1">
-      <c r="B681" s="22"/>
+      <c r="B681" s="23"/>
     </row>
     <row r="682" ht="15.75" customHeight="1">
-      <c r="B682" s="22"/>
+      <c r="B682" s="23"/>
     </row>
     <row r="683" ht="15.75" customHeight="1">
-      <c r="B683" s="22"/>
+      <c r="B683" s="23"/>
     </row>
     <row r="684" ht="15.75" customHeight="1">
-      <c r="B684" s="22"/>
+      <c r="B684" s="23"/>
     </row>
     <row r="685" ht="15.75" customHeight="1">
-      <c r="B685" s="22"/>
+      <c r="B685" s="23"/>
     </row>
     <row r="686" ht="15.75" customHeight="1">
-      <c r="B686" s="22"/>
+      <c r="B686" s="23"/>
     </row>
     <row r="687" ht="15.75" customHeight="1">
-      <c r="B687" s="22"/>
+      <c r="B687" s="23"/>
     </row>
     <row r="688" ht="15.75" customHeight="1">
-      <c r="B688" s="22"/>
+      <c r="B688" s="23"/>
     </row>
     <row r="689" ht="15.75" customHeight="1">
-      <c r="B689" s="22"/>
+      <c r="B689" s="23"/>
     </row>
     <row r="690" ht="15.75" customHeight="1">
-      <c r="B690" s="22"/>
+      <c r="B690" s="23"/>
     </row>
     <row r="691" ht="15.75" customHeight="1">
-      <c r="B691" s="22"/>
+      <c r="B691" s="23"/>
     </row>
     <row r="692" ht="15.75" customHeight="1">
-      <c r="B692" s="22"/>
+      <c r="B692" s="23"/>
     </row>
     <row r="693" ht="15.75" customHeight="1">
-      <c r="B693" s="22"/>
+      <c r="B693" s="23"/>
     </row>
     <row r="694" ht="15.75" customHeight="1">
-      <c r="B694" s="22"/>
+      <c r="B694" s="23"/>
     </row>
     <row r="695" ht="15.75" customHeight="1">
-      <c r="B695" s="22"/>
+      <c r="B695" s="23"/>
     </row>
     <row r="696" ht="15.75" customHeight="1">
-      <c r="B696" s="22"/>
+      <c r="B696" s="23"/>
     </row>
     <row r="697" ht="15.75" customHeight="1">
-      <c r="B697" s="22"/>
+      <c r="B697" s="23"/>
     </row>
     <row r="698" ht="15.75" customHeight="1">
-      <c r="B698" s="22"/>
+      <c r="B698" s="23"/>
     </row>
     <row r="699" ht="15.75" customHeight="1">
-      <c r="B699" s="22"/>
+      <c r="B699" s="23"/>
     </row>
     <row r="700" ht="15.75" customHeight="1">
-      <c r="B700" s="22"/>
+      <c r="B700" s="23"/>
     </row>
     <row r="701" ht="15.75" customHeight="1">
-      <c r="B701" s="22"/>
+      <c r="B701" s="23"/>
     </row>
     <row r="702" ht="15.75" customHeight="1">
-      <c r="B702" s="22"/>
+      <c r="B702" s="23"/>
     </row>
     <row r="703" ht="15.75" customHeight="1">
-      <c r="B703" s="22"/>
+      <c r="B703" s="23"/>
     </row>
     <row r="704" ht="15.75" customHeight="1">
-      <c r="B704" s="22"/>
+      <c r="B704" s="23"/>
     </row>
     <row r="705" ht="15.75" customHeight="1">
-      <c r="B705" s="22"/>
+      <c r="B705" s="23"/>
     </row>
     <row r="706" ht="15.75" customHeight="1">
-      <c r="B706" s="22"/>
+      <c r="B706" s="23"/>
     </row>
     <row r="707" ht="15.75" customHeight="1">
-      <c r="B707" s="22"/>
+      <c r="B707" s="23"/>
     </row>
     <row r="708" ht="15.75" customHeight="1">
-      <c r="B708" s="22"/>
+      <c r="B708" s="23"/>
     </row>
     <row r="709" ht="15.75" customHeight="1">
-      <c r="B709" s="22"/>
+      <c r="B709" s="23"/>
     </row>
     <row r="710" ht="15.75" customHeight="1">
-      <c r="B710" s="22"/>
+      <c r="B710" s="23"/>
     </row>
     <row r="711" ht="15.75" customHeight="1">
-      <c r="B711" s="22"/>
+      <c r="B711" s="23"/>
     </row>
     <row r="712" ht="15.75" customHeight="1">
-      <c r="B712" s="22"/>
+      <c r="B712" s="23"/>
     </row>
     <row r="713" ht="15.75" customHeight="1">
-      <c r="B713" s="22"/>
+      <c r="B713" s="23"/>
     </row>
     <row r="714" ht="15.75" customHeight="1">
-      <c r="B714" s="22"/>
+      <c r="B714" s="23"/>
     </row>
     <row r="715" ht="15.75" customHeight="1">
-      <c r="B715" s="22"/>
+      <c r="B715" s="23"/>
     </row>
     <row r="716" ht="15.75" customHeight="1">
-      <c r="B716" s="22"/>
+      <c r="B716" s="23"/>
     </row>
     <row r="717" ht="15.75" customHeight="1">
-      <c r="B717" s="22"/>
+      <c r="B717" s="23"/>
     </row>
     <row r="718" ht="15.75" customHeight="1">
-      <c r="B718" s="22"/>
+      <c r="B718" s="23"/>
     </row>
     <row r="719" ht="15.75" customHeight="1">
-      <c r="B719" s="22"/>
+      <c r="B719" s="23"/>
     </row>
     <row r="720" ht="15.75" customHeight="1">
-      <c r="B720" s="22"/>
+      <c r="B720" s="23"/>
     </row>
     <row r="721" ht="15.75" customHeight="1">
-      <c r="B721" s="22"/>
+      <c r="B721" s="23"/>
     </row>
     <row r="722" ht="15.75" customHeight="1">
-      <c r="B722" s="22"/>
+      <c r="B722" s="23"/>
     </row>
     <row r="723" ht="15.75" customHeight="1">
-      <c r="B723" s="22"/>
+      <c r="B723" s="23"/>
     </row>
     <row r="724" ht="15.75" customHeight="1">
-      <c r="B724" s="22"/>
+      <c r="B724" s="23"/>
     </row>
     <row r="725" ht="15.75" customHeight="1">
-      <c r="B725" s="22"/>
+      <c r="B725" s="23"/>
     </row>
     <row r="726" ht="15.75" customHeight="1">
-      <c r="B726" s="22"/>
+      <c r="B726" s="23"/>
     </row>
     <row r="727" ht="15.75" customHeight="1">
-      <c r="B727" s="22"/>
+      <c r="B727" s="23"/>
     </row>
     <row r="728" ht="15.75" customHeight="1">
-      <c r="B728" s="22"/>
+      <c r="B728" s="23"/>
     </row>
     <row r="729" ht="15.75" customHeight="1">
-      <c r="B729" s="22"/>
+      <c r="B729" s="23"/>
     </row>
     <row r="730" ht="15.75" customHeight="1">
-      <c r="B730" s="22"/>
+      <c r="B730" s="23"/>
     </row>
     <row r="731" ht="15.75" customHeight="1">
-      <c r="B731" s="22"/>
+      <c r="B731" s="23"/>
     </row>
     <row r="732" ht="15.75" customHeight="1">
-      <c r="B732" s="22"/>
+      <c r="B732" s="23"/>
     </row>
     <row r="733" ht="15.75" customHeight="1">
-      <c r="B733" s="22"/>
+      <c r="B733" s="23"/>
     </row>
     <row r="734" ht="15.75" customHeight="1">
-      <c r="B734" s="22"/>
+      <c r="B734" s="23"/>
     </row>
     <row r="735" ht="15.75" customHeight="1">
-      <c r="B735" s="22"/>
+      <c r="B735" s="23"/>
     </row>
     <row r="736" ht="15.75" customHeight="1">
-      <c r="B736" s="22"/>
+      <c r="B736" s="23"/>
     </row>
     <row r="737" ht="15.75" customHeight="1">
-      <c r="B737" s="22"/>
+      <c r="B737" s="23"/>
     </row>
     <row r="738" ht="15.75" customHeight="1">
-      <c r="B738" s="22"/>
+      <c r="B738" s="23"/>
     </row>
     <row r="739" ht="15.75" customHeight="1">
-      <c r="B739" s="22"/>
+      <c r="B739" s="23"/>
     </row>
     <row r="740" ht="15.75" customHeight="1">
-      <c r="B740" s="22"/>
+      <c r="B740" s="23"/>
     </row>
     <row r="741" ht="15.75" customHeight="1">
-      <c r="B741" s="22"/>
+      <c r="B741" s="23"/>
     </row>
     <row r="742" ht="15.75" customHeight="1">
-      <c r="B742" s="22"/>
+      <c r="B742" s="23"/>
     </row>
     <row r="743" ht="15.75" customHeight="1">
-      <c r="B743" s="22"/>
+      <c r="B743" s="23"/>
     </row>
     <row r="744" ht="15.75" customHeight="1">
-      <c r="B744" s="22"/>
+      <c r="B744" s="23"/>
     </row>
     <row r="745" ht="15.75" customHeight="1">
-      <c r="B745" s="22"/>
+      <c r="B745" s="23"/>
     </row>
     <row r="746" ht="15.75" customHeight="1">
-      <c r="B746" s="22"/>
+      <c r="B746" s="23"/>
     </row>
     <row r="747" ht="15.75" customHeight="1">
-      <c r="B747" s="22"/>
+      <c r="B747" s="23"/>
     </row>
     <row r="748" ht="15.75" customHeight="1">
-      <c r="B748" s="22"/>
+      <c r="B748" s="23"/>
     </row>
     <row r="749" ht="15.75" customHeight="1">
-      <c r="B749" s="22"/>
+      <c r="B749" s="23"/>
     </row>
     <row r="750" ht="15.75" customHeight="1">
-      <c r="B750" s="22"/>
+      <c r="B750" s="23"/>
     </row>
     <row r="751" ht="15.75" customHeight="1">
-      <c r="B751" s="22"/>
+      <c r="B751" s="23"/>
     </row>
     <row r="752" ht="15.75" customHeight="1">
-      <c r="B752" s="22"/>
+      <c r="B752" s="23"/>
     </row>
     <row r="753" ht="15.75" customHeight="1">
-      <c r="B753" s="22"/>
+      <c r="B753" s="23"/>
     </row>
     <row r="754" ht="15.75" customHeight="1">
-      <c r="B754" s="22"/>
+      <c r="B754" s="23"/>
     </row>
     <row r="755" ht="15.75" customHeight="1">
-      <c r="B755" s="22"/>
+      <c r="B755" s="23"/>
     </row>
     <row r="756" ht="15.75" customHeight="1">
-      <c r="B756" s="22"/>
+      <c r="B756" s="23"/>
     </row>
     <row r="757" ht="15.75" customHeight="1">
-      <c r="B757" s="22"/>
+      <c r="B757" s="23"/>
     </row>
     <row r="758" ht="15.75" customHeight="1">
-      <c r="B758" s="22"/>
+      <c r="B758" s="23"/>
     </row>
     <row r="759" ht="15.75" customHeight="1">
-      <c r="B759" s="22"/>
+      <c r="B759" s="23"/>
     </row>
     <row r="760" ht="15.75" customHeight="1">
-      <c r="B760" s="22"/>
+      <c r="B760" s="23"/>
     </row>
     <row r="761" ht="15.75" customHeight="1">
-      <c r="B761" s="22"/>
+      <c r="B761" s="23"/>
     </row>
     <row r="762" ht="15.75" customHeight="1">
-      <c r="B762" s="22"/>
+      <c r="B762" s="23"/>
     </row>
     <row r="763" ht="15.75" customHeight="1">
-      <c r="B763" s="22"/>
+      <c r="B763" s="23"/>
     </row>
     <row r="764" ht="15.75" customHeight="1">
-      <c r="B764" s="22"/>
+      <c r="B764" s="23"/>
     </row>
     <row r="765" ht="15.75" customHeight="1">
-      <c r="B765" s="22"/>
+      <c r="B765" s="23"/>
     </row>
     <row r="766" ht="15.75" customHeight="1">
-      <c r="B766" s="22"/>
+      <c r="B766" s="23"/>
     </row>
     <row r="767" ht="15.75" customHeight="1">
-      <c r="B767" s="22"/>
+      <c r="B767" s="23"/>
     </row>
     <row r="768" ht="15.75" customHeight="1">
-      <c r="B768" s="22"/>
+      <c r="B768" s="23"/>
     </row>
     <row r="769" ht="15.75" customHeight="1">
-      <c r="B769" s="22"/>
+      <c r="B769" s="23"/>
     </row>
     <row r="770" ht="15.75" customHeight="1">
-      <c r="B770" s="22"/>
+      <c r="B770" s="23"/>
     </row>
     <row r="771" ht="15.75" customHeight="1">
-      <c r="B771" s="22"/>
+      <c r="B771" s="23"/>
     </row>
     <row r="772" ht="15.75" customHeight="1">
-      <c r="B772" s="22"/>
+      <c r="B772" s="23"/>
     </row>
     <row r="773" ht="15.75" customHeight="1">
-      <c r="B773" s="22"/>
+      <c r="B773" s="23"/>
     </row>
     <row r="774" ht="15.75" customHeight="1">
-      <c r="B774" s="22"/>
+      <c r="B774" s="23"/>
     </row>
     <row r="775" ht="15.75" customHeight="1">
-      <c r="B775" s="22"/>
+      <c r="B775" s="23"/>
     </row>
     <row r="776" ht="15.75" customHeight="1">
-      <c r="B776" s="22"/>
+      <c r="B776" s="23"/>
     </row>
     <row r="777" ht="15.75" customHeight="1">
-      <c r="B777" s="22"/>
+      <c r="B777" s="23"/>
     </row>
     <row r="778" ht="15.75" customHeight="1">
-      <c r="B778" s="22"/>
+      <c r="B778" s="23"/>
     </row>
     <row r="779" ht="15.75" customHeight="1">
-      <c r="B779" s="22"/>
+      <c r="B779" s="23"/>
     </row>
     <row r="780" ht="15.75" customHeight="1">
-      <c r="B780" s="22"/>
+      <c r="B780" s="23"/>
     </row>
     <row r="781" ht="15.75" customHeight="1">
-      <c r="B781" s="22"/>
+      <c r="B781" s="23"/>
     </row>
     <row r="782" ht="15.75" customHeight="1">
-      <c r="B782" s="22"/>
+      <c r="B782" s="23"/>
     </row>
     <row r="783" ht="15.75" customHeight="1">
-      <c r="B783" s="22"/>
+      <c r="B783" s="23"/>
     </row>
     <row r="784" ht="15.75" customHeight="1">
-      <c r="B784" s="22"/>
+      <c r="B784" s="23"/>
     </row>
     <row r="785" ht="15.75" customHeight="1">
-      <c r="B785" s="22"/>
+      <c r="B785" s="23"/>
     </row>
     <row r="786" ht="15.75" customHeight="1">
-      <c r="B786" s="22"/>
+      <c r="B786" s="23"/>
     </row>
     <row r="787" ht="15.75" customHeight="1">
-      <c r="B787" s="22"/>
+      <c r="B787" s="23"/>
     </row>
     <row r="788" ht="15.75" customHeight="1">
-      <c r="B788" s="22"/>
+      <c r="B788" s="23"/>
     </row>
     <row r="789" ht="15.75" customHeight="1">
-      <c r="B789" s="22"/>
+      <c r="B789" s="23"/>
     </row>
     <row r="790" ht="15.75" customHeight="1">
-      <c r="B790" s="22"/>
+      <c r="B790" s="23"/>
     </row>
     <row r="791" ht="15.75" customHeight="1">
-      <c r="B791" s="22"/>
+      <c r="B791" s="23"/>
     </row>
     <row r="792" ht="15.75" customHeight="1">
-      <c r="B792" s="22"/>
+      <c r="B792" s="23"/>
     </row>
     <row r="793" ht="15.75" customHeight="1">
-      <c r="B793" s="22"/>
+      <c r="B793" s="23"/>
     </row>
     <row r="794" ht="15.75" customHeight="1">
-      <c r="B794" s="22"/>
+      <c r="B794" s="23"/>
     </row>
     <row r="795" ht="15.75" customHeight="1">
-      <c r="B795" s="22"/>
+      <c r="B795" s="23"/>
     </row>
     <row r="796" ht="15.75" customHeight="1">
-      <c r="B796" s="22"/>
+      <c r="B796" s="23"/>
     </row>
     <row r="797" ht="15.75" customHeight="1">
-      <c r="B797" s="22"/>
+      <c r="B797" s="23"/>
     </row>
     <row r="798" ht="15.75" customHeight="1">
-      <c r="B798" s="22"/>
+      <c r="B798" s="23"/>
     </row>
     <row r="799" ht="15.75" customHeight="1">
-      <c r="B799" s="22"/>
+      <c r="B799" s="23"/>
     </row>
     <row r="800" ht="15.75" customHeight="1">
-      <c r="B800" s="22"/>
+      <c r="B800" s="23"/>
     </row>
     <row r="801" ht="15.75" customHeight="1">
-      <c r="B801" s="22"/>
+      <c r="B801" s="23"/>
     </row>
     <row r="802" ht="15.75" customHeight="1">
-      <c r="B802" s="22"/>
+      <c r="B802" s="23"/>
     </row>
     <row r="803" ht="15.75" customHeight="1">
-      <c r="B803" s="22"/>
+      <c r="B803" s="23"/>
     </row>
     <row r="804" ht="15.75" customHeight="1">
-      <c r="B804" s="22"/>
+      <c r="B804" s="23"/>
     </row>
     <row r="805" ht="15.75" customHeight="1">
-      <c r="B805" s="22"/>
+      <c r="B805" s="23"/>
     </row>
     <row r="806" ht="15.75" customHeight="1">
-      <c r="B806" s="22"/>
+      <c r="B806" s="23"/>
     </row>
     <row r="807" ht="15.75" customHeight="1">
-      <c r="B807" s="22"/>
+      <c r="B807" s="23"/>
     </row>
     <row r="808" ht="15.75" customHeight="1">
-      <c r="B808" s="22"/>
+      <c r="B808" s="23"/>
     </row>
     <row r="809" ht="15.75" customHeight="1">
-      <c r="B809" s="22"/>
+      <c r="B809" s="23"/>
     </row>
     <row r="810" ht="15.75" customHeight="1">
-      <c r="B810" s="22"/>
+      <c r="B810" s="23"/>
     </row>
     <row r="811" ht="15.75" customHeight="1">
-      <c r="B811" s="22"/>
+      <c r="B811" s="23"/>
     </row>
     <row r="812" ht="15.75" customHeight="1">
-      <c r="B812" s="22"/>
+      <c r="B812" s="23"/>
     </row>
     <row r="813" ht="15.75" customHeight="1">
-      <c r="B813" s="22"/>
+      <c r="B813" s="23"/>
     </row>
     <row r="814" ht="15.75" customHeight="1">
-      <c r="B814" s="22"/>
+      <c r="B814" s="23"/>
     </row>
     <row r="815" ht="15.75" customHeight="1">
-      <c r="B815" s="22"/>
+      <c r="B815" s="23"/>
     </row>
     <row r="816" ht="15.75" customHeight="1">
-      <c r="B816" s="22"/>
+      <c r="B816" s="23"/>
     </row>
     <row r="817" ht="15.75" customHeight="1">
-      <c r="B817" s="22"/>
+      <c r="B817" s="23"/>
     </row>
     <row r="818" ht="15.75" customHeight="1">
-      <c r="B818" s="22"/>
+      <c r="B818" s="23"/>
     </row>
     <row r="819" ht="15.75" customHeight="1">
-      <c r="B819" s="22"/>
+      <c r="B819" s="23"/>
     </row>
     <row r="820" ht="15.75" customHeight="1">
-      <c r="B820" s="22"/>
+      <c r="B820" s="23"/>
     </row>
     <row r="821" ht="15.75" customHeight="1">
-      <c r="B821" s="22"/>
+      <c r="B821" s="23"/>
     </row>
     <row r="822" ht="15.75" customHeight="1">
-      <c r="B822" s="22"/>
+      <c r="B822" s="23"/>
     </row>
     <row r="823" ht="15.75" customHeight="1">
-      <c r="B823" s="22"/>
+      <c r="B823" s="23"/>
     </row>
     <row r="824" ht="15.75" customHeight="1">
-      <c r="B824" s="22"/>
+      <c r="B824" s="23"/>
     </row>
     <row r="825" ht="15.75" customHeight="1">
-      <c r="B825" s="22"/>
+      <c r="B825" s="23"/>
     </row>
     <row r="826" ht="15.75" customHeight="1">
-      <c r="B826" s="22"/>
+      <c r="B826" s="23"/>
     </row>
     <row r="827" ht="15.75" customHeight="1">
-      <c r="B827" s="22"/>
+      <c r="B827" s="23"/>
     </row>
     <row r="828" ht="15.75" customHeight="1">
-      <c r="B828" s="22"/>
+      <c r="B828" s="23"/>
     </row>
     <row r="829" ht="15.75" customHeight="1">
-      <c r="B829" s="22"/>
+      <c r="B829" s="23"/>
     </row>
     <row r="830" ht="15.75" customHeight="1">
-      <c r="B830" s="22"/>
+      <c r="B830" s="23"/>
     </row>
     <row r="831" ht="15.75" customHeight="1">
-      <c r="B831" s="22"/>
+      <c r="B831" s="23"/>
     </row>
     <row r="832" ht="15.75" customHeight="1">
-      <c r="B832" s="22"/>
+      <c r="B832" s="23"/>
     </row>
     <row r="833" ht="15.75" customHeight="1">
-      <c r="B833" s="22"/>
+      <c r="B833" s="23"/>
     </row>
     <row r="834" ht="15.75" customHeight="1">
-      <c r="B834" s="22"/>
+      <c r="B834" s="23"/>
     </row>
     <row r="835" ht="15.75" customHeight="1">
-      <c r="B835" s="22"/>
+      <c r="B835" s="23"/>
     </row>
     <row r="836" ht="15.75" customHeight="1">
-      <c r="B836" s="22"/>
+      <c r="B836" s="23"/>
     </row>
     <row r="837" ht="15.75" customHeight="1">
-      <c r="B837" s="22"/>
+      <c r="B837" s="23"/>
     </row>
     <row r="838" ht="15.75" customHeight="1">
-      <c r="B838" s="22"/>
+      <c r="B838" s="23"/>
     </row>
     <row r="839" ht="15.75" customHeight="1">
-      <c r="B839" s="22"/>
+      <c r="B839" s="23"/>
     </row>
     <row r="840" ht="15.75" customHeight="1">
-      <c r="B840" s="22"/>
+      <c r="B840" s="23"/>
     </row>
     <row r="841" ht="15.75" customHeight="1">
-      <c r="B841" s="22"/>
+      <c r="B841" s="23"/>
     </row>
     <row r="842" ht="15.75" customHeight="1">
-      <c r="B842" s="22"/>
+      <c r="B842" s="23"/>
     </row>
     <row r="843" ht="15.75" customHeight="1">
-      <c r="B843" s="22"/>
+      <c r="B843" s="23"/>
     </row>
     <row r="844" ht="15.75" customHeight="1">
-      <c r="B844" s="22"/>
+      <c r="B844" s="23"/>
     </row>
     <row r="845" ht="15.75" customHeight="1">
-      <c r="B845" s="22"/>
+      <c r="B845" s="23"/>
     </row>
     <row r="846" ht="15.75" customHeight="1">
-      <c r="B846" s="22"/>
+      <c r="B846" s="23"/>
     </row>
     <row r="847" ht="15.75" customHeight="1">
-      <c r="B847" s="22"/>
+      <c r="B847" s="23"/>
     </row>
     <row r="848" ht="15.75" customHeight="1">
-      <c r="B848" s="22"/>
+      <c r="B848" s="23"/>
     </row>
     <row r="849" ht="15.75" customHeight="1">
-      <c r="B849" s="22"/>
+      <c r="B849" s="23"/>
     </row>
     <row r="850" ht="15.75" customHeight="1">
-      <c r="B850" s="22"/>
+      <c r="B850" s="23"/>
     </row>
     <row r="851" ht="15.75" customHeight="1">
-      <c r="B851" s="22"/>
+      <c r="B851" s="23"/>
     </row>
     <row r="852" ht="15.75" customHeight="1">
-      <c r="B852" s="22"/>
+      <c r="B852" s="23"/>
     </row>
     <row r="853" ht="15.75" customHeight="1">
-      <c r="B853" s="22"/>
+      <c r="B853" s="23"/>
     </row>
     <row r="854" ht="15.75" customHeight="1">
-      <c r="B854" s="22"/>
+      <c r="B854" s="23"/>
     </row>
     <row r="855" ht="15.75" customHeight="1">
-      <c r="B855" s="22"/>
+      <c r="B855" s="23"/>
     </row>
     <row r="856" ht="15.75" customHeight="1">
-      <c r="B856" s="22"/>
+      <c r="B856" s="23"/>
     </row>
     <row r="857" ht="15.75" customHeight="1">
-      <c r="B857" s="22"/>
+      <c r="B857" s="23"/>
     </row>
     <row r="858" ht="15.75" customHeight="1">
-      <c r="B858" s="22"/>
+      <c r="B858" s="23"/>
     </row>
     <row r="859" ht="15.75" customHeight="1">
-      <c r="B859" s="22"/>
+      <c r="B859" s="23"/>
     </row>
     <row r="860" ht="15.75" customHeight="1">
-      <c r="B860" s="22"/>
+      <c r="B860" s="23"/>
     </row>
     <row r="861" ht="15.75" customHeight="1">
-      <c r="B861" s="22"/>
+      <c r="B861" s="23"/>
     </row>
     <row r="862" ht="15.75" customHeight="1">
-      <c r="B862" s="22"/>
+      <c r="B862" s="23"/>
     </row>
     <row r="863" ht="15.75" customHeight="1">
-      <c r="B863" s="22"/>
+      <c r="B863" s="23"/>
     </row>
     <row r="864" ht="15.75" customHeight="1">
-      <c r="B864" s="22"/>
+      <c r="B864" s="23"/>
     </row>
     <row r="865" ht="15.75" customHeight="1">
-      <c r="B865" s="22"/>
+      <c r="B865" s="23"/>
     </row>
     <row r="866" ht="15.75" customHeight="1">
-      <c r="B866" s="22"/>
+      <c r="B866" s="23"/>
     </row>
     <row r="867" ht="15.75" customHeight="1">
-      <c r="B867" s="22"/>
+      <c r="B867" s="23"/>
     </row>
     <row r="868" ht="15.75" customHeight="1">
-      <c r="B868" s="22"/>
+      <c r="B868" s="23"/>
     </row>
     <row r="869" ht="15.75" customHeight="1">
-      <c r="B869" s="22"/>
+      <c r="B869" s="23"/>
     </row>
     <row r="870" ht="15.75" customHeight="1">
-      <c r="B870" s="22"/>
+      <c r="B870" s="23"/>
     </row>
     <row r="871" ht="15.75" customHeight="1">
-      <c r="B871" s="22"/>
+      <c r="B871" s="23"/>
     </row>
     <row r="872" ht="15.75" customHeight="1">
-      <c r="B872" s="22"/>
+      <c r="B872" s="23"/>
     </row>
     <row r="873" ht="15.75" customHeight="1">
-      <c r="B873" s="22"/>
+      <c r="B873" s="23"/>
     </row>
     <row r="874" ht="15.75" customHeight="1">
-      <c r="B874" s="22"/>
+      <c r="B874" s="23"/>
     </row>
     <row r="875" ht="15.75" customHeight="1">
-      <c r="B875" s="22"/>
+      <c r="B875" s="23"/>
     </row>
     <row r="876" ht="15.75" customHeight="1">
-      <c r="B876" s="22"/>
+      <c r="B876" s="23"/>
     </row>
     <row r="877" ht="15.75" customHeight="1">
-      <c r="B877" s="22"/>
+      <c r="B877" s="23"/>
     </row>
     <row r="878" ht="15.75" customHeight="1">
-      <c r="B878" s="22"/>
+      <c r="B878" s="23"/>
     </row>
     <row r="879" ht="15.75" customHeight="1">
-      <c r="B879" s="22"/>
+      <c r="B879" s="23"/>
     </row>
     <row r="880" ht="15.75" customHeight="1">
-      <c r="B880" s="22"/>
+      <c r="B880" s="23"/>
     </row>
     <row r="881" ht="15.75" customHeight="1">
-      <c r="B881" s="22"/>
+      <c r="B881" s="23"/>
     </row>
     <row r="882" ht="15.75" customHeight="1">
-      <c r="B882" s="22"/>
+      <c r="B882" s="23"/>
     </row>
     <row r="883" ht="15.75" customHeight="1">
-      <c r="B883" s="22"/>
+      <c r="B883" s="23"/>
     </row>
     <row r="884" ht="15.75" customHeight="1">
-      <c r="B884" s="22"/>
+      <c r="B884" s="23"/>
     </row>
     <row r="885" ht="15.75" customHeight="1">
-      <c r="B885" s="22"/>
+      <c r="B885" s="23"/>
     </row>
     <row r="886" ht="15.75" customHeight="1">
-      <c r="B886" s="22"/>
+      <c r="B886" s="23"/>
     </row>
     <row r="887" ht="15.75" customHeight="1">
-      <c r="B887" s="22"/>
+      <c r="B887" s="23"/>
     </row>
     <row r="888" ht="15.75" customHeight="1">
-      <c r="B888" s="22"/>
+      <c r="B888" s="23"/>
     </row>
     <row r="889" ht="15.75" customHeight="1">
-      <c r="B889" s="22"/>
+      <c r="B889" s="23"/>
     </row>
     <row r="890" ht="15.75" customHeight="1">
-      <c r="B890" s="22"/>
+      <c r="B890" s="23"/>
     </row>
     <row r="891" ht="15.75" customHeight="1">
-      <c r="B891" s="22"/>
+      <c r="B891" s="23"/>
     </row>
     <row r="892" ht="15.75" customHeight="1">
-      <c r="B892" s="22"/>
+      <c r="B892" s="23"/>
     </row>
     <row r="893" ht="15.75" customHeight="1">
-      <c r="B893" s="22"/>
+      <c r="B893" s="23"/>
     </row>
     <row r="894" ht="15.75" customHeight="1">
-      <c r="B894" s="22"/>
+      <c r="B894" s="23"/>
     </row>
     <row r="895" ht="15.75" customHeight="1">
-      <c r="B895" s="22"/>
+      <c r="B895" s="23"/>
     </row>
     <row r="896" ht="15.75" customHeight="1">
-      <c r="B896" s="22"/>
+      <c r="B896" s="23"/>
     </row>
     <row r="897" ht="15.75" customHeight="1">
-      <c r="B897" s="22"/>
+      <c r="B897" s="23"/>
     </row>
     <row r="898" ht="15.75" customHeight="1">
-      <c r="B898" s="22"/>
+      <c r="B898" s="23"/>
     </row>
     <row r="899" ht="15.75" customHeight="1">
-      <c r="B899" s="22"/>
+      <c r="B899" s="23"/>
     </row>
     <row r="900" ht="15.75" customHeight="1">
-      <c r="B900" s="22"/>
+      <c r="B900" s="23"/>
     </row>
     <row r="901" ht="15.75" customHeight="1">
-      <c r="B901" s="22"/>
+      <c r="B901" s="23"/>
     </row>
     <row r="902" ht="15.75" customHeight="1">
-      <c r="B902" s="22"/>
+      <c r="B902" s="23"/>
     </row>
     <row r="903" ht="15.75" customHeight="1">
-      <c r="B903" s="22"/>
+      <c r="B903" s="23"/>
     </row>
     <row r="904" ht="15.75" customHeight="1">
-      <c r="B904" s="22"/>
+      <c r="B904" s="23"/>
     </row>
     <row r="905" ht="15.75" customHeight="1">
-      <c r="B905" s="22"/>
+      <c r="B905" s="23"/>
     </row>
     <row r="906" ht="15.75" customHeight="1">
-      <c r="B906" s="22"/>
+      <c r="B906" s="23"/>
     </row>
     <row r="907" ht="15.75" customHeight="1">
-      <c r="B907" s="22"/>
+      <c r="B907" s="23"/>
     </row>
     <row r="908" ht="15.75" customHeight="1">
-      <c r="B908" s="22"/>
+      <c r="B908" s="23"/>
     </row>
     <row r="909" ht="15.75" customHeight="1">
-      <c r="B909" s="22"/>
+      <c r="B909" s="23"/>
     </row>
     <row r="910" ht="15.75" customHeight="1">
-      <c r="B910" s="22"/>
+      <c r="B910" s="23"/>
     </row>
     <row r="911" ht="15.75" customHeight="1">
-      <c r="B911" s="22"/>
+      <c r="B911" s="23"/>
     </row>
     <row r="912" ht="15.75" customHeight="1">
-      <c r="B912" s="22"/>
+      <c r="B912" s="23"/>
     </row>
     <row r="913" ht="15.75" customHeight="1">
-      <c r="B913" s="22"/>
+      <c r="B913" s="23"/>
     </row>
     <row r="914" ht="15.75" customHeight="1">
-      <c r="B914" s="22"/>
+      <c r="B914" s="23"/>
     </row>
     <row r="915" ht="15.75" customHeight="1">
-      <c r="B915" s="22"/>
+      <c r="B915" s="23"/>
     </row>
     <row r="916" ht="15.75" customHeight="1">
-      <c r="B916" s="22"/>
+      <c r="B916" s="23"/>
     </row>
     <row r="917" ht="15.75" customHeight="1">
-      <c r="B917" s="22"/>
+      <c r="B917" s="23"/>
     </row>
     <row r="918" ht="15.75" customHeight="1">
-      <c r="B918" s="22"/>
+      <c r="B918" s="23"/>
     </row>
     <row r="919" ht="15.75" customHeight="1">
-      <c r="B919" s="22"/>
+      <c r="B919" s="23"/>
     </row>
     <row r="920" ht="15.75" customHeight="1">
-      <c r="B920" s="22"/>
+      <c r="B920" s="23"/>
     </row>
     <row r="921" ht="15.75" customHeight="1">
-      <c r="B921" s="22"/>
+      <c r="B921" s="23"/>
     </row>
     <row r="922" ht="15.75" customHeight="1">
-      <c r="B922" s="22"/>
+      <c r="B922" s="23"/>
     </row>
     <row r="923" ht="15.75" customHeight="1">
-      <c r="B923" s="22"/>
+      <c r="B923" s="23"/>
     </row>
     <row r="924" ht="15.75" customHeight="1">
-      <c r="B924" s="22"/>
+      <c r="B924" s="23"/>
     </row>
     <row r="925" ht="15.75" customHeight="1">
-      <c r="B925" s="22"/>
+      <c r="B925" s="23"/>
     </row>
     <row r="926" ht="15.75" customHeight="1">
-      <c r="B926" s="22"/>
+      <c r="B926" s="23"/>
     </row>
     <row r="927" ht="15.75" customHeight="1">
-      <c r="B927" s="22"/>
+      <c r="B927" s="23"/>
     </row>
     <row r="928" ht="15.75" customHeight="1">
-      <c r="B928" s="22"/>
+      <c r="B928" s="23"/>
     </row>
     <row r="929" ht="15.75" customHeight="1">
-      <c r="B929" s="22"/>
+      <c r="B929" s="23"/>
     </row>
     <row r="930" ht="15.75" customHeight="1">
-      <c r="B930" s="22"/>
+      <c r="B930" s="23"/>
     </row>
     <row r="931" ht="15.75" customHeight="1">
-      <c r="B931" s="22"/>
+      <c r="B931" s="23"/>
     </row>
     <row r="932" ht="15.75" customHeight="1">
-      <c r="B932" s="22"/>
+      <c r="B932" s="23"/>
     </row>
     <row r="933" ht="15.75" customHeight="1">
-      <c r="B933" s="22"/>
+      <c r="B933" s="23"/>
     </row>
     <row r="934" ht="15.75" customHeight="1">
-      <c r="B934" s="22"/>
+      <c r="B934" s="23"/>
     </row>
     <row r="935" ht="15.75" customHeight="1">
-      <c r="B935" s="22"/>
+      <c r="B935" s="23"/>
     </row>
     <row r="936" ht="15.75" customHeight="1">
-      <c r="B936" s="22"/>
+      <c r="B936" s="23"/>
     </row>
     <row r="937" ht="15.75" customHeight="1">
-      <c r="B937" s="22"/>
+      <c r="B937" s="23"/>
     </row>
     <row r="938" ht="15.75" customHeight="1">
-      <c r="B938" s="22"/>
+      <c r="B938" s="23"/>
     </row>
     <row r="939" ht="15.75" customHeight="1">
-      <c r="B939" s="22"/>
+      <c r="B939" s="23"/>
     </row>
     <row r="940" ht="15.75" customHeight="1">
-      <c r="B940" s="22"/>
+      <c r="B940" s="23"/>
     </row>
     <row r="941" ht="15.75" customHeight="1">
-      <c r="B941" s="22"/>
+      <c r="B941" s="23"/>
     </row>
     <row r="942" ht="15.75" customHeight="1">
-      <c r="B942" s="22"/>
+      <c r="B942" s="23"/>
     </row>
     <row r="943" ht="15.75" customHeight="1">
-      <c r="B943" s="22"/>
+      <c r="B943" s="23"/>
     </row>
     <row r="944" ht="15.75" customHeight="1">
-      <c r="B944" s="22"/>
+      <c r="B944" s="23"/>
     </row>
     <row r="945" ht="15.75" customHeight="1">
-      <c r="B945" s="22"/>
+      <c r="B945" s="23"/>
     </row>
     <row r="946" ht="15.75" customHeight="1">
-      <c r="B946" s="22"/>
+      <c r="B946" s="23"/>
     </row>
     <row r="947" ht="15.75" customHeight="1">
-      <c r="B947" s="22"/>
+      <c r="B947" s="23"/>
     </row>
     <row r="948" ht="15.75" customHeight="1">
-      <c r="B948" s="22"/>
+      <c r="B948" s="23"/>
     </row>
     <row r="949" ht="15.75" customHeight="1">
-      <c r="B949" s="22"/>
+      <c r="B949" s="23"/>
     </row>
     <row r="950" ht="15.75" customHeight="1">
-      <c r="B950" s="22"/>
+      <c r="B950" s="23"/>
     </row>
     <row r="951" ht="15.75" customHeight="1">
-      <c r="B951" s="22"/>
+      <c r="B951" s="23"/>
     </row>
     <row r="952" ht="15.75" customHeight="1">
-      <c r="B952" s="22"/>
+      <c r="B952" s="23"/>
     </row>
     <row r="953" ht="15.75" customHeight="1">
-      <c r="B953" s="22"/>
+      <c r="B953" s="23"/>
     </row>
     <row r="954" ht="15.75" customHeight="1">
-      <c r="B954" s="22"/>
+      <c r="B954" s="23"/>
     </row>
     <row r="955" ht="15.75" customHeight="1">
-      <c r="B955" s="22"/>
+      <c r="B955" s="23"/>
     </row>
     <row r="956" ht="15.75" customHeight="1">
-      <c r="B956" s="22"/>
+      <c r="B956" s="23"/>
     </row>
     <row r="957" ht="15.75" customHeight="1">
-      <c r="B957" s="22"/>
+      <c r="B957" s="23"/>
     </row>
     <row r="958" ht="15.75" customHeight="1">
-      <c r="B958" s="22"/>
+      <c r="B958" s="23"/>
     </row>
     <row r="959" ht="15.75" customHeight="1">
-      <c r="B959" s="22"/>
+      <c r="B959" s="23"/>
     </row>
     <row r="960" ht="15.75" customHeight="1">
-      <c r="B960" s="22"/>
+      <c r="B960" s="23"/>
     </row>
     <row r="961" ht="15.75" customHeight="1">
-      <c r="B961" s="22"/>
+      <c r="B961" s="23"/>
     </row>
     <row r="962" ht="15.75" customHeight="1">
-      <c r="B962" s="22"/>
+      <c r="B962" s="23"/>
     </row>
     <row r="963" ht="15.75" customHeight="1">
-      <c r="B963" s="22"/>
+      <c r="B963" s="23"/>
     </row>
     <row r="964" ht="15.75" customHeight="1">
-      <c r="B964" s="22"/>
+      <c r="B964" s="23"/>
     </row>
     <row r="965" ht="15.75" customHeight="1">
-      <c r="B965" s="22"/>
+      <c r="B965" s="23"/>
     </row>
     <row r="966" ht="15.75" customHeight="1">
-      <c r="B966" s="22"/>
+      <c r="B966" s="23"/>
     </row>
     <row r="967" ht="15.75" customHeight="1">
-      <c r="B967" s="22"/>
+      <c r="B967" s="23"/>
     </row>
     <row r="968" ht="15.75" customHeight="1">
-      <c r="B968" s="22"/>
+      <c r="B968" s="23"/>
     </row>
     <row r="969" ht="15.75" customHeight="1">
-      <c r="B969" s="22"/>
+      <c r="B969" s="23"/>
     </row>
     <row r="970" ht="15.75" customHeight="1">
-      <c r="B970" s="22"/>
+      <c r="B970" s="23"/>
     </row>
     <row r="971" ht="15.75" customHeight="1">
-      <c r="B971" s="22"/>
+      <c r="B971" s="23"/>
     </row>
     <row r="972" ht="15.75" customHeight="1">
-      <c r="B972" s="22"/>
+      <c r="B972" s="23"/>
     </row>
     <row r="973" ht="15.75" customHeight="1">
-      <c r="B973" s="22"/>
+      <c r="B973" s="23"/>
     </row>
     <row r="974" ht="15.75" customHeight="1">
-      <c r="B974" s="22"/>
+      <c r="B974" s="23"/>
     </row>
     <row r="975" ht="15.75" customHeight="1">
-      <c r="B975" s="22"/>
+      <c r="B975" s="23"/>
     </row>
     <row r="976" ht="15.75" customHeight="1">
-      <c r="B976" s="22"/>
+      <c r="B976" s="23"/>
     </row>
     <row r="977" ht="15.75" customHeight="1">
-      <c r="B977" s="22"/>
+      <c r="B977" s="23"/>
     </row>
     <row r="978" ht="15.75" customHeight="1">
-      <c r="B978" s="22"/>
+      <c r="B978" s="23"/>
     </row>
     <row r="979" ht="15.75" customHeight="1">
-      <c r="B979" s="22"/>
+      <c r="B979" s="23"/>
     </row>
     <row r="980" ht="15.75" customHeight="1">
-      <c r="B980" s="22"/>
+      <c r="B980" s="23"/>
     </row>
     <row r="981" ht="15.75" customHeight="1">
-      <c r="B981" s="22"/>
+      <c r="B981" s="23"/>
     </row>
     <row r="982" ht="15.75" customHeight="1">
-      <c r="B982" s="22"/>
+      <c r="B982" s="23"/>
     </row>
     <row r="983" ht="15.75" customHeight="1">
-      <c r="B983" s="22"/>
+      <c r="B983" s="23"/>
     </row>
     <row r="984" ht="15.75" customHeight="1">
-      <c r="B984" s="22"/>
+      <c r="B984" s="23"/>
     </row>
     <row r="985" ht="15.75" customHeight="1">
-      <c r="B985" s="22"/>
+      <c r="B985" s="23"/>
     </row>
     <row r="986" ht="15.75" customHeight="1">
-      <c r="B986" s="22"/>
+      <c r="B986" s="23"/>
     </row>
     <row r="987" ht="15.75" customHeight="1">
-      <c r="B987" s="22"/>
+      <c r="B987" s="23"/>
     </row>
     <row r="988" ht="15.75" customHeight="1">
-      <c r="B988" s="22"/>
+      <c r="B988" s="23"/>
     </row>
     <row r="989" ht="15.75" customHeight="1">
-      <c r="B989" s="22"/>
+      <c r="B989" s="23"/>
     </row>
     <row r="990" ht="15.75" customHeight="1">
-      <c r="B990" s="22"/>
+      <c r="B990" s="23"/>
     </row>
     <row r="991" ht="15.75" customHeight="1">
-      <c r="B991" s="22"/>
+      <c r="B991" s="23"/>
     </row>
     <row r="992" ht="15.75" customHeight="1">
-      <c r="B992" s="22"/>
+      <c r="B992" s="23"/>
     </row>
     <row r="993" ht="15.75" customHeight="1">
-      <c r="B993" s="22"/>
+      <c r="B993" s="23"/>
     </row>
     <row r="994" ht="15.75" customHeight="1">
-      <c r="B994" s="22"/>
+      <c r="B994" s="23"/>
     </row>
     <row r="995" ht="15.75" customHeight="1">
-      <c r="B995" s="22"/>
+      <c r="B995" s="23"/>
     </row>
     <row r="996" ht="15.75" customHeight="1">
-      <c r="B996" s="22"/>
+      <c r="B996" s="23"/>
     </row>
     <row r="997" ht="15.75" customHeight="1">
-      <c r="B997" s="22"/>
+      <c r="B997" s="23"/>
     </row>
     <row r="998" ht="15.75" customHeight="1">
-      <c r="B998" s="22"/>
+      <c r="B998" s="23"/>
     </row>
     <row r="999" ht="15.75" customHeight="1">
-      <c r="B999" s="22"/>
+      <c r="B999" s="23"/>
     </row>
     <row r="1000" ht="15.75" customHeight="1">
-      <c r="B1000" s="22"/>
+      <c r="B1000" s="23"/>
+    </row>
+    <row r="1001" ht="15.75" customHeight="1">
+      <c r="B1001" s="23"/>
+    </row>
+    <row r="1002" ht="15.75" customHeight="1">
+      <c r="B1002" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>